<commit_message>
Add - recopilación de métricas y uso de Jupyter Lab
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FCC399-E918-4184-92F0-D7A22B1AC305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02DF484-2BFF-4168-A3F2-2DCDFC4C0010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -84,13 +84,73 @@
   </si>
   <si>
     <t>CPU</t>
+  </si>
+  <si>
+    <t>Unidad de Procesamiento</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>modelo 2</t>
+  </si>
+  <si>
+    <t>modelo 4</t>
+  </si>
+  <si>
+    <t>modelo 8</t>
+  </si>
+  <si>
+    <t>modelo 3</t>
+  </si>
+  <si>
+    <t>modelo 5</t>
+  </si>
+  <si>
+    <t>modelo 6</t>
+  </si>
+  <si>
+    <t>modelo 7</t>
+  </si>
+  <si>
+    <t>modelo 9</t>
+  </si>
+  <si>
+    <t>modelo 10</t>
+  </si>
+  <si>
+    <t>modelo 11</t>
+  </si>
+  <si>
+    <t>modelo 12</t>
+  </si>
+  <si>
+    <t>modelo 13</t>
+  </si>
+  <si>
+    <t>modelo 14</t>
+  </si>
+  <si>
+    <t>modelo 15</t>
+  </si>
+  <si>
+    <t>modelo 16</t>
+  </si>
+  <si>
+    <t>modelo 17</t>
+  </si>
+  <si>
+    <t>modelo 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +181,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,12 +216,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -165,8 +226,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECEECE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,42 +286,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,6 +413,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFECEECE"/>
       <color rgb="FF17891A"/>
     </mruColors>
   </colors>
@@ -567,10 +748,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:P8"/>
+  <dimension ref="B2:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,147 +764,734 @@
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
     <col min="14" max="14" width="4.42578125" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="10" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="P4" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="11">
+        <v>1E-4</v>
+      </c>
+      <c r="D5" s="11">
         <v>200</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="11">
         <v>16</v>
       </c>
-      <c r="F5" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="11">
         <v>100</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="2">
+      <c r="H5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="12">
         <v>0.54179999999999995</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="12">
         <v>0.73829999999999996</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="12">
         <v>0.52149999999999996</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="12">
         <v>0.72629999999999995</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="2">
+      <c r="N5" s="2"/>
+      <c r="O5" s="12">
         <v>71.400000000000006</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="2"/>
+      <c r="B6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>200</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="2"/>
+      <c r="B7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="15">
+        <v>200</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="16">
+        <v>0.2407</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0.22650000000000001</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0.44390000000000002</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
+      <c r="B8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="19">
+        <v>200</v>
+      </c>
+      <c r="E8" s="8">
+        <v>8</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="20">
+        <v>0.23219999999999999</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0.2359</v>
+      </c>
+      <c r="M8" s="20">
+        <v>0.46079999999999999</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="19">
+        <v>200</v>
+      </c>
+      <c r="E9" s="8">
+        <v>16</v>
+      </c>
+      <c r="F9" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="19">
+        <v>0.2727</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0.55230000000000001</v>
+      </c>
+      <c r="L9" s="19">
+        <v>0.26419999999999999</v>
+      </c>
+      <c r="M9" s="19">
+        <v>0.54920000000000002</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="9">
+        <v>100</v>
+      </c>
+      <c r="E10" s="24">
+        <v>4</v>
+      </c>
+      <c r="F10" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="24">
+        <v>0.2329</v>
+      </c>
+      <c r="K10" s="24">
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="L10" s="24">
+        <v>0.216</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0.42409999999999998</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="P10" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1E-4</v>
+      </c>
+      <c r="D11" s="9">
+        <v>300</v>
+      </c>
+      <c r="E11" s="24">
+        <v>4</v>
+      </c>
+      <c r="F11" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="24">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="K11" s="24">
+        <v>0.42170000000000002</v>
+      </c>
+      <c r="L11" s="24">
+        <v>0.20519999999999999</v>
+      </c>
+      <c r="M11" s="24">
+        <v>0.40229999999999999</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="24">
+        <v>5.5</v>
+      </c>
+      <c r="P11" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1E-4</v>
+      </c>
+      <c r="D12" s="9">
+        <v>400</v>
+      </c>
+      <c r="E12" s="24">
+        <v>4</v>
+      </c>
+      <c r="F12" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="24">
+        <v>0.21460000000000001</v>
+      </c>
+      <c r="K12" s="24">
+        <v>0.41930000000000001</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="M12" s="24">
+        <v>0.375</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="24">
+        <v>7.4</v>
+      </c>
+      <c r="P12" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="27">
+        <v>1E-4</v>
+      </c>
+      <c r="D13" s="28">
+        <v>500</v>
+      </c>
+      <c r="E13" s="27">
+        <v>4</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="27">
+        <v>0.22589999999999999</v>
+      </c>
+      <c r="K13" s="27">
+        <v>0.45029999999999998</v>
+      </c>
+      <c r="L13" s="27">
+        <v>0.20860000000000001</v>
+      </c>
+      <c r="M13" s="27">
+        <v>0.4037</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="P13" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="29">
+        <v>1E-4</v>
+      </c>
+      <c r="D14" s="9">
+        <v>100</v>
+      </c>
+      <c r="E14" s="29">
+        <v>8</v>
+      </c>
+      <c r="F14" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="29">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="K14" s="29">
+        <v>0.44979999999999998</v>
+      </c>
+      <c r="L14" s="29">
+        <v>0.2132</v>
+      </c>
+      <c r="M14" s="29">
+        <v>0.40060000000000001</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="29">
+        <v>1.7</v>
+      </c>
+      <c r="P14" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1E-4</v>
+      </c>
+      <c r="D15" s="9">
+        <v>300</v>
+      </c>
+      <c r="E15" s="29">
+        <v>8</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="29">
+        <v>0.23369999999999999</v>
+      </c>
+      <c r="K15" s="29">
+        <v>0.45979999999999999</v>
+      </c>
+      <c r="L15" s="29">
+        <v>0.216</v>
+      </c>
+      <c r="M15" s="29">
+        <v>0.40529999999999999</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="29">
+        <v>5.2</v>
+      </c>
+      <c r="P15" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="29">
+        <v>1E-4</v>
+      </c>
+      <c r="D16" s="9">
+        <v>400</v>
+      </c>
+      <c r="E16" s="29">
+        <v>8</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="29">
+        <v>0.24440000000000001</v>
+      </c>
+      <c r="K16" s="29">
+        <v>0.4763</v>
+      </c>
+      <c r="L16" s="29">
+        <v>0.23130000000000001</v>
+      </c>
+      <c r="M16" s="29">
+        <v>0.44169999999999998</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="29">
+        <v>7.1</v>
+      </c>
+      <c r="P16" s="30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="31">
+        <v>1E-4</v>
+      </c>
+      <c r="D17" s="28">
+        <v>500</v>
+      </c>
+      <c r="E17" s="31">
+        <v>8</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="31">
+        <v>0.2369</v>
+      </c>
+      <c r="K17" s="31">
+        <v>0.46039999999999998</v>
+      </c>
+      <c r="L17" s="31">
+        <v>0.2205</v>
+      </c>
+      <c r="M17" s="31">
+        <v>0.41849999999999998</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="31">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="P17" s="32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="33">
+        <v>1E-4</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33">
+        <v>16</v>
+      </c>
+      <c r="F18" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="33">
+        <v>1E-4</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33">
+        <v>16</v>
+      </c>
+      <c r="F19" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="33">
+        <v>1E-4</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33">
+        <v>16</v>
+      </c>
+      <c r="F20" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="33">
+        <v>1E-4</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33">
+        <v>16</v>
+      </c>
+      <c r="F21" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="33">
+        <v>1E-4</v>
+      </c>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33">
+        <v>16</v>
+      </c>
+      <c r="F22" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f>104/60</f>
+        <v>1.7333333333333334</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add - avance de grilla(métricas de la red)
Se probó con eliminar la regulación l2 en la red. al parecer el error baja considerablemente. El gráfico de errores NMSE se puede visualizar más estable.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02DF484-2BFF-4168-A3F2-2DCDFC4C0010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4995C0AF-457D-4E92-AF73-FEF2CDEF187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -144,13 +144,25 @@
   </si>
   <si>
     <t>modelo 18</t>
+  </si>
+  <si>
+    <t>modelo 19</t>
+  </si>
+  <si>
+    <t>modelo 20</t>
+  </si>
+  <si>
+    <t>modelo 21</t>
+  </si>
+  <si>
+    <t>modelo 22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +179,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +189,19 @@
     <font>
       <sz val="11"/>
       <color theme="6"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,24 +321,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -339,10 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,10 +363,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,46 +375,68 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -748,10 +782,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:P26"/>
+  <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,19 +796,24 @@
     <col min="5" max="6" width="10" customWidth="1"/>
     <col min="8" max="8" width="9.28515625" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="4.42578125" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+    </row>
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -813,684 +852,1149 @@
       <c r="O4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
-        <v>1E-4</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="C5" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="D5" s="10">
         <v>200</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>16</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>0.01</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>100</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>0.54179999999999995</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>0.73829999999999996</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>0.52149999999999996</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="11">
         <v>0.72629999999999995</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="12">
+      <c r="O5" s="11">
         <v>71.400000000000006</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="P5" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="15">
-        <v>1E-4</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="C6" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="D6" s="13">
         <v>200</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <v>0.01</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17" t="s">
+      <c r="O6" s="14"/>
+      <c r="P6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="15">
-        <v>1E-4</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="C7" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="13">
         <v>200</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>0.01</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="16">
+      <c r="J7" s="14">
         <v>0.2407</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="14">
         <v>0.49049999999999999</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="14">
         <v>0.22650000000000001</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="14">
         <v>0.44390000000000002</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="16">
+      <c r="O7" s="14">
         <v>3.8</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="19">
-        <v>1E-4</v>
-      </c>
-      <c r="D8" s="19">
+      <c r="C8" s="17">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="17">
         <v>200</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>8</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="17">
         <v>0.01</v>
       </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19" t="s">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="20">
+      <c r="J8" s="18">
         <v>0.23219999999999999</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="18">
         <v>0.45900000000000002</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="18">
         <v>0.2359</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="18">
         <v>0.46079999999999999</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="20">
+      <c r="O8" s="18">
         <v>3.6</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="19">
-        <v>1E-4</v>
-      </c>
-      <c r="D9" s="19">
+      <c r="C9" s="17">
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="17">
         <v>200</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>16</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <v>0.01</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19" t="s">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="19">
+      <c r="J9" s="17">
         <v>0.2727</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="17">
         <v>0.55230000000000001</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="17">
         <v>0.26419999999999999</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="17">
         <v>0.54920000000000002</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <v>3.5</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="24">
-        <v>1E-4</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="C10" s="22">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="8">
         <v>100</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="22">
         <v>4</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="22">
         <v>0.01</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="24">
+      <c r="J10" s="22">
         <v>0.2329</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="22">
         <v>0.46639999999999998</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="22">
         <v>0.216</v>
       </c>
-      <c r="M10" s="24">
+      <c r="M10" s="22">
         <v>0.42409999999999998</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="24">
+      <c r="O10" s="22">
         <v>1.8</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="P10" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24">
-        <v>1E-4</v>
-      </c>
-      <c r="D11" s="9">
+      <c r="C11" s="22">
+        <v>1E-4</v>
+      </c>
+      <c r="D11" s="8">
         <v>300</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="22">
         <v>4</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="22">
         <v>0.01</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24" t="s">
+      <c r="G11" s="22"/>
+      <c r="H11" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="24">
+      <c r="J11" s="22">
         <v>0.21970000000000001</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="22">
         <v>0.42170000000000002</v>
       </c>
-      <c r="L11" s="24">
+      <c r="L11" s="22">
         <v>0.20519999999999999</v>
       </c>
-      <c r="M11" s="24">
+      <c r="M11" s="22">
         <v>0.40229999999999999</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="24">
+      <c r="O11" s="22">
         <v>5.5</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="P11" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="24">
-        <v>1E-4</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C12" s="22">
+        <v>1E-4</v>
+      </c>
+      <c r="D12" s="8">
         <v>400</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="22">
         <v>4</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="22">
         <v>0.01</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24" t="s">
+      <c r="G12" s="22"/>
+      <c r="H12" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="24">
-        <v>0.21460000000000001</v>
-      </c>
-      <c r="K12" s="24">
-        <v>0.41930000000000001</v>
-      </c>
-      <c r="L12" s="24">
-        <v>0.19450000000000001</v>
-      </c>
-      <c r="M12" s="24">
-        <v>0.375</v>
+      <c r="J12" s="22">
+        <v>0.2291</v>
+      </c>
+      <c r="K12" s="22">
+        <v>0.4466</v>
+      </c>
+      <c r="L12" s="22">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="M12" s="22">
+        <v>0.41060000000000002</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="24">
-        <v>7.4</v>
-      </c>
-      <c r="P12" s="25" t="s">
+      <c r="O12" s="22">
+        <v>7.2</v>
+      </c>
+      <c r="P12" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="27">
-        <v>1E-4</v>
-      </c>
-      <c r="D13" s="28">
+      <c r="C13" s="24">
+        <v>1E-4</v>
+      </c>
+      <c r="D13" s="25">
         <v>500</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="24">
         <v>4</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="24">
         <v>0.01</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27" t="s">
+      <c r="G13" s="24"/>
+      <c r="H13" s="24" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="27">
+      <c r="J13" s="24">
         <v>0.22589999999999999</v>
       </c>
-      <c r="K13" s="27">
+      <c r="K13" s="24">
         <v>0.45029999999999998</v>
       </c>
-      <c r="L13" s="27">
+      <c r="L13" s="24">
         <v>0.20860000000000001</v>
       </c>
-      <c r="M13" s="27">
+      <c r="M13" s="24">
         <v>0.4037</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="27">
+      <c r="O13" s="24">
         <v>9.3000000000000007</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="29">
-        <v>1E-4</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="C14" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D14" s="8">
         <v>100</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="26">
         <v>8</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="26">
         <v>0.01</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="29">
+      <c r="J14" s="26">
         <v>0.22900000000000001</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="26">
         <v>0.44979999999999998</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="26">
         <v>0.2132</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="26">
         <v>0.40060000000000001</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="29">
+      <c r="O14" s="26">
         <v>1.7</v>
       </c>
-      <c r="P14" s="30" t="s">
+      <c r="P14" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="29">
-        <v>1E-4</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="C15" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D15" s="8">
         <v>300</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="26">
         <v>8</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="26">
         <v>0.01</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="29">
+      <c r="J15" s="26">
         <v>0.23369999999999999</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="26">
         <v>0.45979999999999999</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="26">
         <v>0.216</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="26">
         <v>0.40529999999999999</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="29">
+      <c r="O15" s="26">
         <v>5.2</v>
       </c>
-      <c r="P15" s="30" t="s">
+      <c r="P15" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="29">
-        <v>1E-4</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C16" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D16" s="8">
         <v>400</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="26">
         <v>8</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="26">
         <v>0.01</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29" t="s">
+      <c r="G16" s="26"/>
+      <c r="H16" s="26" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="29">
+      <c r="J16" s="26">
         <v>0.24440000000000001</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="26">
         <v>0.4763</v>
       </c>
-      <c r="L16" s="29">
+      <c r="L16" s="26">
         <v>0.23130000000000001</v>
       </c>
-      <c r="M16" s="29">
+      <c r="M16" s="26">
         <v>0.44169999999999998</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="29">
+      <c r="O16" s="26">
         <v>7.1</v>
       </c>
-      <c r="P16" s="30" t="s">
+      <c r="P16" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="31">
-        <v>1E-4</v>
-      </c>
-      <c r="D17" s="28">
+      <c r="C17" s="28">
+        <v>1E-4</v>
+      </c>
+      <c r="D17" s="25">
         <v>500</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="28">
         <v>8</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="28">
         <v>0.01</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31" t="s">
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="31">
+      <c r="J17" s="28">
         <v>0.2369</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="28">
         <v>0.46039999999999998</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="28">
         <v>0.2205</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="28">
         <v>0.41849999999999998</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="31">
+      <c r="O17" s="28">
         <v>8.8000000000000007</v>
       </c>
-      <c r="P17" s="32" t="s">
+      <c r="P17" s="29" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33">
+      <c r="C18" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D18" s="8">
+        <v>100</v>
+      </c>
+      <c r="E18" s="30">
         <v>16</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="30">
         <v>0.01</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33" t="s">
+      <c r="G18" s="30"/>
+      <c r="H18" s="30" t="s">
         <v>6</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
+      <c r="J18" s="30">
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="K18" s="30">
+        <v>0.62180000000000002</v>
+      </c>
+      <c r="L18" s="30">
+        <v>0.27579999999999999</v>
+      </c>
+      <c r="M18" s="30">
+        <v>0.59919999999999995</v>
+      </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="34" t="s">
+      <c r="O18" s="30">
+        <v>1.8</v>
+      </c>
+      <c r="P18" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33">
+      <c r="C19" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D19" s="8">
+        <v>300</v>
+      </c>
+      <c r="E19" s="30">
         <v>16</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="30">
         <v>0.01</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33" t="s">
+      <c r="G19" s="30"/>
+      <c r="H19" s="30" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
+      <c r="J19" s="30">
+        <v>0.2576</v>
+      </c>
+      <c r="K19" s="30">
+        <v>0.50990000000000002</v>
+      </c>
+      <c r="L19" s="30">
+        <v>0.24279999999999999</v>
+      </c>
+      <c r="M19" s="30">
+        <v>0.48770000000000002</v>
+      </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="34" t="s">
+      <c r="O19" s="30">
+        <v>5.2</v>
+      </c>
+      <c r="P19" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33">
+      <c r="C20" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D20" s="8">
+        <v>400</v>
+      </c>
+      <c r="E20" s="30">
         <v>16</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="30">
         <v>0.01</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33" t="s">
+      <c r="G20" s="30"/>
+      <c r="H20" s="30" t="s">
         <v>6</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
+      <c r="J20" s="30">
+        <v>0.24970000000000001</v>
+      </c>
+      <c r="K20" s="30">
+        <v>0.4894</v>
+      </c>
+      <c r="L20" s="30">
+        <v>0.2356</v>
+      </c>
+      <c r="M20" s="30">
+        <v>0.46839999999999998</v>
+      </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="34" t="s">
+      <c r="O20" s="30">
+        <v>6.8</v>
+      </c>
+      <c r="P20" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33">
+      <c r="C21" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D21" s="8">
+        <v>500</v>
+      </c>
+      <c r="E21" s="30">
         <v>16</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="30">
         <v>0.01</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33" t="s">
+      <c r="G21" s="30"/>
+      <c r="H21" s="30" t="s">
         <v>6</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
+      <c r="J21" s="30">
+        <v>0.2462</v>
+      </c>
+      <c r="K21" s="30">
+        <v>0.47820000000000001</v>
+      </c>
+      <c r="L21" s="30">
+        <v>0.2324</v>
+      </c>
+      <c r="M21" s="30">
+        <v>0.46629999999999999</v>
+      </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="34" t="s">
+      <c r="O21" s="30">
+        <v>8.5</v>
+      </c>
+      <c r="P21" s="31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="33">
-        <v>1E-4</v>
-      </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33">
+      <c r="C23" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="D23" s="6">
+        <v>100</v>
+      </c>
+      <c r="E23" s="36">
+        <v>4</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="D24" s="6">
+        <v>200</v>
+      </c>
+      <c r="E24" s="36">
+        <v>4</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="D25" s="6">
+        <v>300</v>
+      </c>
+      <c r="E25" s="36">
+        <v>4</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="D26" s="6">
+        <v>400</v>
+      </c>
+      <c r="E26" s="36">
+        <v>4</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="36">
+        <v>1E-4</v>
+      </c>
+      <c r="D27" s="6">
+        <v>500</v>
+      </c>
+      <c r="E27" s="36">
+        <v>4</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D28" s="8">
+        <v>100</v>
+      </c>
+      <c r="E28" s="26">
+        <v>8</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D29" s="8">
+        <v>200</v>
+      </c>
+      <c r="E29" s="26">
+        <v>8</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D30" s="8">
+        <v>300</v>
+      </c>
+      <c r="E30" s="26">
+        <v>8</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D31" s="8">
+        <v>400</v>
+      </c>
+      <c r="E31" s="26">
+        <v>8</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="26">
+        <v>1E-4</v>
+      </c>
+      <c r="D32" s="8">
+        <v>500</v>
+      </c>
+      <c r="E32" s="26">
+        <v>8</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D33" s="8">
+        <v>100</v>
+      </c>
+      <c r="E33" s="30">
         <v>16</v>
       </c>
-      <c r="F22" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J26">
-        <f>104/60</f>
-        <v>1.7333333333333334</v>
+      <c r="F33" s="8"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D34" s="8">
+        <v>200</v>
+      </c>
+      <c r="E34" s="30">
+        <v>16</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D35" s="8">
+        <v>300</v>
+      </c>
+      <c r="E35" s="30">
+        <v>16</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="30"/>
+      <c r="P35" s="40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D36" s="8">
+        <v>400</v>
+      </c>
+      <c r="E36" s="30">
+        <v>16</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="30"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="30"/>
+      <c r="P36" s="40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D37" s="8">
+        <v>500</v>
+      </c>
+      <c r="E37" s="30">
+        <v>16</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="30"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="30"/>
+      <c r="P37" s="40" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test - Se modifican la cantidad de filtros de la red al doble
Los filtros por capas se amplifican al doble, es decir de 64 a 128, de 128 a 256 y de 256 a 512. Con ello, se analizará en rendimiento del modelo. Se observó un mejoría de la calidad de los modelo (disminución de loss y NMSE) al eliminar la regulación l2 en las capas de la red, por lo tanto, ahora se mantendrá omitida dicha regulación.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4995C0AF-457D-4E92-AF73-FEF2CDEF187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BD7147-1D0A-45EB-ACE8-234D82142482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="48">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -156,13 +156,41 @@
   </si>
   <si>
     <t>modelo 22</t>
+  </si>
+  <si>
+    <t>orden-filtros-capas: [64,64,128,128,256,256,128,128,128,64,64,64]</t>
+  </si>
+  <si>
+    <t>mejores errores v1.0</t>
+  </si>
+  <si>
+    <t>orden-filtros-capas: [128,128,256,256,512,512,256,256,256,128,128,128]</t>
+  </si>
+  <si>
+    <t>modelo 23</t>
+  </si>
+  <si>
+    <t>modelo 24</t>
+  </si>
+  <si>
+    <t>modelo 25</t>
+  </si>
+  <si>
+    <t>modelo 26</t>
+  </si>
+  <si>
+    <t>modelo 27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,8 +234,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,8 +315,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -317,11 +364,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,18 +407,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,9 +422,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -412,9 +459,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -438,6 +482,100 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,8 +585,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF17891A"/>
       <color rgb="FFECEECE"/>
-      <color rgb="FF17891A"/>
     </mruColors>
   </colors>
   <extLst>
@@ -782,10 +920,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:P37"/>
+  <dimension ref="B2:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,14 +944,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+    </row>
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+    </row>
+    <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -852,7 +1002,7 @@
       <c r="O4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="30" t="s">
         <v>16</v>
       </c>
     </row>
@@ -879,1127 +1029,1513 @@
         <v>6</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="11">
+      <c r="J5" s="39">
         <v>0.54179999999999995</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="39">
         <v>0.73829999999999996</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="39">
         <v>0.52149999999999996</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="39">
         <v>0.72629999999999995</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="11">
+      <c r="O5" s="48">
         <v>71.400000000000006</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="13">
-        <v>1E-4</v>
-      </c>
-      <c r="D6" s="13">
+      <c r="C6" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="D6" s="12">
         <v>200</v>
       </c>
       <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>0.01</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="15" t="s">
+      <c r="O6" s="49"/>
+      <c r="P6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="13">
-        <v>1E-4</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="C7" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="12">
         <v>200</v>
       </c>
       <c r="E7" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>0.01</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="14">
+      <c r="J7" s="40">
         <v>0.2407</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="40">
         <v>0.49049999999999999</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="40">
         <v>0.22650000000000001</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="40">
         <v>0.44390000000000002</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="14">
+      <c r="O7" s="49">
         <v>3.8</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="17">
-        <v>1E-4</v>
-      </c>
-      <c r="D8" s="17">
+      <c r="C8" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="15">
         <v>200</v>
       </c>
       <c r="E8" s="7">
         <v>8</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="15">
         <v>0.01</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="18">
+      <c r="J8" s="38">
         <v>0.23219999999999999</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="38">
         <v>0.45900000000000002</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="38">
         <v>0.2359</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="38">
         <v>0.46079999999999999</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="18">
+      <c r="O8" s="50">
         <v>3.6</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="P8" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="17">
-        <v>1E-4</v>
-      </c>
-      <c r="D9" s="17">
+      <c r="C9" s="15">
+        <v>1E-4</v>
+      </c>
+      <c r="D9" s="15">
         <v>200</v>
       </c>
       <c r="E9" s="7">
         <v>16</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="15">
         <v>0.01</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="17">
+      <c r="J9" s="41">
         <v>0.2727</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="41">
         <v>0.55230000000000001</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="41">
         <v>0.26419999999999999</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="41">
         <v>0.54920000000000002</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="17">
+      <c r="O9" s="51">
         <v>3.5</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="P9" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="19">
         <v>1E-4</v>
       </c>
       <c r="D10" s="8">
         <v>100</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="19">
         <v>4</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="19">
         <v>0.01</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="19"/>
+      <c r="H10" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="22">
+      <c r="J10" s="42">
         <v>0.2329</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="42">
         <v>0.46639999999999998</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="42">
         <v>0.216</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="42">
         <v>0.42409999999999998</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="22">
+      <c r="O10" s="52">
         <v>1.8</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="19">
         <v>1E-4</v>
       </c>
       <c r="D11" s="8">
         <v>300</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="19">
         <v>4</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="19">
         <v>0.01</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22" t="s">
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="22">
+      <c r="J11" s="42">
         <v>0.21970000000000001</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="42">
         <v>0.42170000000000002</v>
       </c>
-      <c r="L11" s="22">
+      <c r="L11" s="42">
         <v>0.20519999999999999</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="42">
         <v>0.40229999999999999</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="22">
+      <c r="O11" s="52">
         <v>5.5</v>
       </c>
-      <c r="P11" s="23" t="s">
+      <c r="P11" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="19">
         <v>1E-4</v>
       </c>
       <c r="D12" s="8">
         <v>400</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="19">
         <v>4</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="19">
         <v>0.01</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22" t="s">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="22">
+      <c r="J12" s="42">
         <v>0.2291</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="42">
         <v>0.4466</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="42">
         <v>0.21240000000000001</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="42">
         <v>0.41060000000000002</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="22">
+      <c r="O12" s="52">
         <v>7.2</v>
       </c>
-      <c r="P12" s="23" t="s">
+      <c r="P12" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="24">
-        <v>1E-4</v>
-      </c>
-      <c r="D13" s="25">
+      <c r="C13" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="D13" s="22">
         <v>500</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="21">
         <v>4</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="21">
         <v>0.01</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="24">
+      <c r="J13" s="43">
         <v>0.22589999999999999</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="43">
         <v>0.45029999999999998</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="43">
         <v>0.20860000000000001</v>
       </c>
-      <c r="M13" s="24">
+      <c r="M13" s="43">
         <v>0.4037</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="24">
+      <c r="O13" s="53">
         <v>9.3000000000000007</v>
       </c>
-      <c r="P13" s="23" t="s">
+      <c r="P13" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="23">
         <v>1E-4</v>
       </c>
       <c r="D14" s="8">
         <v>100</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="23">
         <v>8</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="23">
         <v>0.01</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="23" t="s">
         <v>6</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="26">
+      <c r="J14" s="44">
         <v>0.22900000000000001</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="44">
         <v>0.44979999999999998</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="44">
         <v>0.2132</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="44">
         <v>0.40060000000000001</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="26">
+      <c r="O14" s="54">
         <v>1.7</v>
       </c>
-      <c r="P14" s="27" t="s">
+      <c r="P14" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="23">
         <v>1E-4</v>
       </c>
       <c r="D15" s="8">
         <v>300</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="23">
         <v>8</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="23">
         <v>0.01</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26" t="s">
+      <c r="G15" s="23"/>
+      <c r="H15" s="23" t="s">
         <v>6</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="26">
+      <c r="J15" s="44">
         <v>0.23369999999999999</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="44">
         <v>0.45979999999999999</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L15" s="44">
         <v>0.216</v>
       </c>
-      <c r="M15" s="26">
+      <c r="M15" s="44">
         <v>0.40529999999999999</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="26">
+      <c r="O15" s="54">
         <v>5.2</v>
       </c>
-      <c r="P15" s="27" t="s">
+      <c r="P15" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="23">
         <v>1E-4</v>
       </c>
       <c r="D16" s="8">
         <v>400</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="23">
         <v>8</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="23">
         <v>0.01</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26" t="s">
+      <c r="G16" s="23"/>
+      <c r="H16" s="23" t="s">
         <v>6</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="26">
+      <c r="J16" s="44">
         <v>0.24440000000000001</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="44">
         <v>0.4763</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="44">
         <v>0.23130000000000001</v>
       </c>
-      <c r="M16" s="26">
+      <c r="M16" s="44">
         <v>0.44169999999999998</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="26">
+      <c r="O16" s="54">
         <v>7.1</v>
       </c>
-      <c r="P16" s="27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
+      <c r="P16" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="28">
-        <v>1E-4</v>
-      </c>
-      <c r="D17" s="25">
+      <c r="C17" s="25">
+        <v>1E-4</v>
+      </c>
+      <c r="D17" s="22">
         <v>500</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="25">
         <v>8</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="25">
         <v>0.01</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="25" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="28">
+      <c r="J17" s="45">
         <v>0.2369</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="45">
         <v>0.46039999999999998</v>
       </c>
-      <c r="L17" s="28">
+      <c r="L17" s="45">
         <v>0.2205</v>
       </c>
-      <c r="M17" s="28">
+      <c r="M17" s="45">
         <v>0.41849999999999998</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="28">
+      <c r="O17" s="55">
         <v>8.8000000000000007</v>
       </c>
-      <c r="P17" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="P17" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="27">
         <v>1E-4</v>
       </c>
       <c r="D18" s="8">
         <v>100</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="27">
         <v>16</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="27">
         <v>0.01</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27" t="s">
         <v>6</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="30">
+      <c r="J18" s="46">
         <v>0.29420000000000002</v>
       </c>
-      <c r="K18" s="30">
+      <c r="K18" s="46">
         <v>0.62180000000000002</v>
       </c>
-      <c r="L18" s="30">
+      <c r="L18" s="46">
         <v>0.27579999999999999</v>
       </c>
-      <c r="M18" s="30">
+      <c r="M18" s="46">
         <v>0.59919999999999995</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="30">
+      <c r="O18" s="56">
         <v>1.8</v>
       </c>
-      <c r="P18" s="31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
+      <c r="P18" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="27">
         <v>1E-4</v>
       </c>
       <c r="D19" s="8">
         <v>300</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="27">
         <v>16</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="27">
         <v>0.01</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30" t="s">
+      <c r="G19" s="27"/>
+      <c r="H19" s="27" t="s">
         <v>6</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="30">
+      <c r="J19" s="46">
         <v>0.2576</v>
       </c>
-      <c r="K19" s="30">
+      <c r="K19" s="46">
         <v>0.50990000000000002</v>
       </c>
-      <c r="L19" s="30">
+      <c r="L19" s="46">
         <v>0.24279999999999999</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="46">
         <v>0.48770000000000002</v>
       </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="30">
+      <c r="O19" s="56">
         <v>5.2</v>
       </c>
-      <c r="P19" s="31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="P19" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="27">
         <v>1E-4</v>
       </c>
       <c r="D20" s="8">
         <v>400</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="27">
         <v>16</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="27">
         <v>0.01</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="27"/>
+      <c r="H20" s="27" t="s">
         <v>6</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="30">
+      <c r="J20" s="46">
         <v>0.24970000000000001</v>
       </c>
-      <c r="K20" s="30">
+      <c r="K20" s="46">
         <v>0.4894</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="46">
         <v>0.2356</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M20" s="46">
         <v>0.46839999999999998</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="30">
+      <c r="O20" s="56">
         <v>6.8</v>
       </c>
-      <c r="P20" s="31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="P20" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="27">
         <v>1E-4</v>
       </c>
       <c r="D21" s="8">
         <v>500</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="27">
         <v>16</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="27">
         <v>0.01</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30" t="s">
+      <c r="G21" s="27"/>
+      <c r="H21" s="27" t="s">
         <v>6</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="30">
+      <c r="J21" s="46">
         <v>0.2462</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="46">
         <v>0.47820000000000001</v>
       </c>
-      <c r="L21" s="30">
+      <c r="L21" s="46">
         <v>0.2324</v>
       </c>
-      <c r="M21" s="30">
+      <c r="M21" s="46">
         <v>0.46629999999999999</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="30">
+      <c r="O21" s="56">
         <v>8.5</v>
       </c>
-      <c r="P21" s="31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="P21" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="33"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="32">
         <v>1E-4</v>
       </c>
       <c r="D23" s="6">
         <v>100</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="32">
         <v>4</v>
       </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36" t="s">
+      <c r="G23" s="32"/>
+      <c r="H23" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
+      <c r="J23" s="47">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="K23" s="47">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="L23" s="47">
+        <v>5.6399999999999999E-2</v>
+      </c>
+      <c r="M23" s="47">
+        <v>0.12939999999999999</v>
+      </c>
       <c r="N23" s="2"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="O23" s="58">
+        <v>1.8</v>
+      </c>
+      <c r="P23" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q23" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="R23" s="61"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="32">
         <v>1E-4</v>
       </c>
       <c r="D24" s="6">
         <v>200</v>
       </c>
-      <c r="E24" s="36">
+      <c r="E24" s="32">
         <v>4</v>
       </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36" t="s">
+      <c r="G24" s="32"/>
+      <c r="H24" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
+      <c r="J24" s="47">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="K24" s="47">
+        <v>8.6E-3</v>
+      </c>
+      <c r="L24" s="47">
+        <v>5.62E-2</v>
+      </c>
+      <c r="M24" s="47">
+        <v>0.1293</v>
+      </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
+      <c r="O24" s="58">
+        <v>3.6</v>
+      </c>
+      <c r="P24" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="61"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="36">
+      <c r="C25" s="32">
         <v>1E-4</v>
       </c>
       <c r="D25" s="6">
         <v>300</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="32">
         <v>4</v>
       </c>
       <c r="F25" s="6"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36" t="s">
+      <c r="G25" s="32"/>
+      <c r="H25" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
+      <c r="J25" s="47">
+        <v>1.4E-3</v>
+      </c>
+      <c r="K25" s="47">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L25" s="47">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="M25" s="47">
+        <v>0.1212</v>
+      </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
+      <c r="O25" s="58">
+        <v>5.4</v>
+      </c>
+      <c r="P25" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="60"/>
+      <c r="R25" s="61"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="32">
         <v>1E-4</v>
       </c>
       <c r="D26" s="6">
         <v>400</v>
       </c>
-      <c r="E26" s="36">
+      <c r="E26" s="32">
         <v>4</v>
       </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36" t="s">
+      <c r="G26" s="32"/>
+      <c r="H26" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
+      <c r="J26" s="47">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K26" s="47">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="L26" s="47">
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="M26" s="47">
+        <v>0.1237</v>
+      </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
+      <c r="O26" s="58">
+        <v>7.2</v>
+      </c>
+      <c r="P26" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26" s="60"/>
+      <c r="R26" s="61"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="32">
         <v>1E-4</v>
       </c>
       <c r="D27" s="6">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="32">
         <v>4</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36" t="s">
+      <c r="G27" s="32"/>
+      <c r="H27" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="J27" s="47">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="K27" s="47">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="L27" s="47">
+        <v>5.62E-2</v>
+      </c>
+      <c r="M27" s="47">
+        <v>0.12820000000000001</v>
+      </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
+      <c r="O27" s="58">
+        <v>8.9</v>
+      </c>
+      <c r="P27" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="61"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="23">
         <v>1E-4</v>
       </c>
       <c r="D28" s="8">
         <v>100</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="23">
         <v>8</v>
       </c>
       <c r="F28" s="8"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="36" t="s">
+      <c r="G28" s="23"/>
+      <c r="H28" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I28" s="2"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
+      <c r="J28" s="44">
+        <v>7.6E-3</v>
+      </c>
+      <c r="K28" s="44">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="L28" s="44">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="M28" s="44">
+        <v>0.12180000000000001</v>
+      </c>
       <c r="N28" s="2"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="21" t="s">
+      <c r="O28" s="54">
+        <v>1.8</v>
+      </c>
+      <c r="P28" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="61"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="23">
         <v>1E-4</v>
       </c>
       <c r="D29" s="8">
         <v>200</v>
       </c>
-      <c r="E29" s="26">
+      <c r="E29" s="23">
         <v>8</v>
       </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="36" t="s">
+      <c r="G29" s="23"/>
+      <c r="H29" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
+      <c r="J29" s="44">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="K29" s="44">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="L29" s="44">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="M29" s="44">
+        <v>0.1138</v>
+      </c>
       <c r="N29" s="2"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="21" t="s">
+      <c r="O29" s="54">
+        <v>3.6</v>
+      </c>
+      <c r="P29" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="61"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="23">
         <v>1E-4</v>
       </c>
       <c r="D30" s="8">
         <v>300</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E30" s="23">
         <v>8</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="36" t="s">
+      <c r="G30" s="23"/>
+      <c r="H30" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
+      <c r="J30" s="44">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K30" s="44">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="L30" s="44">
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="M30" s="44">
+        <v>0.1149</v>
+      </c>
       <c r="N30" s="2"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="21" t="s">
+      <c r="O30" s="54">
+        <v>5.3</v>
+      </c>
+      <c r="P30" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="61"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="23">
         <v>1E-4</v>
       </c>
       <c r="D31" s="8">
         <v>400</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="23">
         <v>8</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="36" t="s">
+      <c r="G31" s="23"/>
+      <c r="H31" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I31" s="2"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
+      <c r="J31" s="44">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K31" s="44">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="L31" s="44">
+        <v>6.1400000000000003E-2</v>
+      </c>
+      <c r="M31" s="44">
+        <v>0.1221</v>
+      </c>
       <c r="N31" s="2"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="s">
+      <c r="O31" s="54">
+        <v>7</v>
+      </c>
+      <c r="P31" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="61"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="23">
         <v>1E-4</v>
       </c>
       <c r="D32" s="8">
         <v>500</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="23">
         <v>8</v>
       </c>
       <c r="F32" s="8"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="36" t="s">
+      <c r="G32" s="23"/>
+      <c r="H32" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I32" s="2"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
+      <c r="J32" s="44">
+        <v>9.3041E-4</v>
+      </c>
+      <c r="K32" s="44">
+        <v>2.3E-3</v>
+      </c>
+      <c r="L32" s="44">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="M32" s="44">
+        <v>0.1167</v>
+      </c>
       <c r="N32" s="2"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="39" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="21" t="s">
+      <c r="O32" s="54">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="P32" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="61"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="30">
+      <c r="C33" s="27">
         <v>1E-4</v>
       </c>
       <c r="D33" s="8">
         <v>100</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="27">
         <v>16</v>
       </c>
       <c r="F33" s="8"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="36" t="s">
+      <c r="G33" s="27"/>
+      <c r="H33" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I33" s="2"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
+      <c r="J33" s="46">
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="K33" s="46">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="L33" s="46">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="M33" s="46">
+        <v>0.16020000000000001</v>
+      </c>
       <c r="N33" s="2"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="21" t="s">
+      <c r="O33" s="56">
+        <v>1.8</v>
+      </c>
+      <c r="P33" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="61"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="27">
         <v>1E-4</v>
       </c>
       <c r="D34" s="8">
         <v>200</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="27">
         <v>16</v>
       </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="36" t="s">
+      <c r="G34" s="27"/>
+      <c r="H34" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I34" s="2"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
+      <c r="J34" s="46">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="K34" s="46">
+        <v>1.78E-2</v>
+      </c>
+      <c r="L34" s="46">
+        <v>6.1499999999999999E-2</v>
+      </c>
+      <c r="M34" s="46">
+        <v>0.16550000000000001</v>
+      </c>
       <c r="N34" s="2"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="21" t="s">
+      <c r="O34" s="56">
+        <v>3.5</v>
+      </c>
+      <c r="P34" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="61"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C35" s="27">
         <v>1E-4</v>
       </c>
       <c r="D35" s="8">
         <v>300</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="27">
         <v>16</v>
       </c>
       <c r="F35" s="8"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="36" t="s">
+      <c r="G35" s="27"/>
+      <c r="H35" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
+      <c r="J35" s="46">
+        <v>3.3E-3</v>
+      </c>
+      <c r="K35" s="46">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="L35" s="46">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="M35" s="46">
+        <v>0.1643</v>
+      </c>
       <c r="N35" s="2"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="21" t="s">
+      <c r="O35" s="56">
+        <v>5.2</v>
+      </c>
+      <c r="P35" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="61"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="27">
         <v>1E-4</v>
       </c>
       <c r="D36" s="8">
         <v>400</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="27">
         <v>16</v>
       </c>
       <c r="F36" s="8"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="36" t="s">
+      <c r="G36" s="27"/>
+      <c r="H36" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I36" s="2"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
+      <c r="J36" s="46">
+        <v>2E-3</v>
+      </c>
+      <c r="K36" s="46">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L36" s="46">
+        <v>5.9200000000000003E-2</v>
+      </c>
+      <c r="M36" s="46">
+        <v>0.1593</v>
+      </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="s">
+      <c r="O36" s="56">
+        <v>6.9</v>
+      </c>
+      <c r="P36" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="61"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="27">
         <v>1E-4</v>
       </c>
       <c r="D37" s="8">
         <v>500</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="27">
         <v>16</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="36" t="s">
+      <c r="G37" s="27"/>
+      <c r="H37" s="32" t="s">
         <v>6</v>
       </c>
       <c r="I37" s="2"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
+      <c r="J37" s="46">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="K37" s="46">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L37" s="46">
+        <v>5.8900000000000001E-2</v>
+      </c>
+      <c r="M37" s="46">
+        <v>0.15870000000000001</v>
+      </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="40" t="s">
+      <c r="O37" s="56">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="P37" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="61"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="68"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+    </row>
+    <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="65" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="L40" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="N40" s="2"/>
+      <c r="O40" s="66" t="s">
+        <v>14</v>
+      </c>
+      <c r="P40" s="67" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="D41" s="6">
+        <v>100</v>
+      </c>
+      <c r="E41" s="32">
+        <v>4</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B42" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="D42" s="6">
+        <v>200</v>
+      </c>
+      <c r="E42" s="32">
+        <v>4</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="D43" s="6">
+        <v>300</v>
+      </c>
+      <c r="E43" s="32">
+        <v>4</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="32"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="D44" s="6">
+        <v>400</v>
+      </c>
+      <c r="E44" s="32">
+        <v>4</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="32">
+        <v>1E-3</v>
+      </c>
+      <c r="D45" s="6">
+        <v>500</v>
+      </c>
+      <c r="E45" s="32">
+        <v>4</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="34" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="Q23:R37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test- avance métricas con filtros amplificados al doble
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BD7147-1D0A-45EB-ACE8-234D82142482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CC0947-99BA-41AB-9DBE-5D6671F4F8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="4230" yWindow="6390" windowWidth="21600" windowHeight="7155" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -180,6 +180,21 @@
   </si>
   <si>
     <t>modelo 27</t>
+  </si>
+  <si>
+    <t>modelo 28</t>
+  </si>
+  <si>
+    <t>modelo 29</t>
+  </si>
+  <si>
+    <t>modelo 30</t>
+  </si>
+  <si>
+    <t>modelo 31</t>
+  </si>
+  <si>
+    <t>modelo 32</t>
   </si>
 </sst>
 </file>
@@ -190,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +252,20 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -377,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -483,9 +512,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -547,36 +573,59 @@
     <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,10 +969,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:R45"/>
+  <dimension ref="B2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,24 +993,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1029,20 +1078,20 @@
         <v>6</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="39">
+      <c r="J5" s="38">
         <v>0.54179999999999995</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="38">
         <v>0.73829999999999996</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="38">
         <v>0.52149999999999996</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="38">
         <v>0.72629999999999995</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="48">
+      <c r="O5" s="47">
         <v>71.400000000000006</v>
       </c>
       <c r="P5" s="31" t="s">
@@ -1070,12 +1119,12 @@
         <v>6</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="49"/>
+      <c r="O6" s="48"/>
       <c r="P6" s="13" t="s">
         <v>17</v>
       </c>
@@ -1101,20 +1150,20 @@
         <v>6</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="40">
+      <c r="J7" s="39">
         <v>0.2407</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="39">
         <v>0.49049999999999999</v>
       </c>
-      <c r="L7" s="40">
+      <c r="L7" s="39">
         <v>0.22650000000000001</v>
       </c>
-      <c r="M7" s="40">
+      <c r="M7" s="39">
         <v>0.44390000000000002</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="49">
+      <c r="O7" s="48">
         <v>3.8</v>
       </c>
       <c r="P7" s="13" t="s">
@@ -1142,20 +1191,20 @@
         <v>18</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="38">
+      <c r="J8" s="37">
         <v>0.23219999999999999</v>
       </c>
-      <c r="K8" s="38">
+      <c r="K8" s="37">
         <v>0.45900000000000002</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="37">
         <v>0.2359</v>
       </c>
-      <c r="M8" s="38">
+      <c r="M8" s="37">
         <v>0.46079999999999999</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="50">
+      <c r="O8" s="49">
         <v>3.6</v>
       </c>
       <c r="P8" s="16" t="s">
@@ -1183,20 +1232,20 @@
         <v>6</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="41">
+      <c r="J9" s="40">
         <v>0.2727</v>
       </c>
-      <c r="K9" s="41">
+      <c r="K9" s="40">
         <v>0.55230000000000001</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="40">
         <v>0.26419999999999999</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="40">
         <v>0.54920000000000002</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="51">
+      <c r="O9" s="50">
         <v>3.5</v>
       </c>
       <c r="P9" s="16" t="s">
@@ -1224,20 +1273,20 @@
         <v>6</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="42">
+      <c r="J10" s="41">
         <v>0.2329</v>
       </c>
-      <c r="K10" s="42">
+      <c r="K10" s="41">
         <v>0.46639999999999998</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="41">
         <v>0.216</v>
       </c>
-      <c r="M10" s="42">
+      <c r="M10" s="41">
         <v>0.42409999999999998</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="52">
+      <c r="O10" s="51">
         <v>1.8</v>
       </c>
       <c r="P10" s="20" t="s">
@@ -1265,20 +1314,20 @@
         <v>6</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="42">
+      <c r="J11" s="41">
         <v>0.21970000000000001</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="41">
         <v>0.42170000000000002</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="41">
         <v>0.20519999999999999</v>
       </c>
-      <c r="M11" s="42">
+      <c r="M11" s="41">
         <v>0.40229999999999999</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="52">
+      <c r="O11" s="51">
         <v>5.5</v>
       </c>
       <c r="P11" s="20" t="s">
@@ -1306,20 +1355,20 @@
         <v>6</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="42">
+      <c r="J12" s="41">
         <v>0.2291</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="41">
         <v>0.4466</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="41">
         <v>0.21240000000000001</v>
       </c>
-      <c r="M12" s="42">
+      <c r="M12" s="41">
         <v>0.41060000000000002</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="52">
+      <c r="O12" s="51">
         <v>7.2</v>
       </c>
       <c r="P12" s="20" t="s">
@@ -1347,20 +1396,20 @@
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="43">
+      <c r="J13" s="42">
         <v>0.22589999999999999</v>
       </c>
-      <c r="K13" s="43">
+      <c r="K13" s="42">
         <v>0.45029999999999998</v>
       </c>
-      <c r="L13" s="43">
+      <c r="L13" s="42">
         <v>0.20860000000000001</v>
       </c>
-      <c r="M13" s="43">
+      <c r="M13" s="42">
         <v>0.4037</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="53">
+      <c r="O13" s="52">
         <v>9.3000000000000007</v>
       </c>
       <c r="P13" s="20" t="s">
@@ -1388,20 +1437,20 @@
         <v>6</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="44">
+      <c r="J14" s="43">
         <v>0.22900000000000001</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="43">
         <v>0.44979999999999998</v>
       </c>
-      <c r="L14" s="44">
+      <c r="L14" s="43">
         <v>0.2132</v>
       </c>
-      <c r="M14" s="44">
+      <c r="M14" s="43">
         <v>0.40060000000000001</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="54">
+      <c r="O14" s="53">
         <v>1.7</v>
       </c>
       <c r="P14" s="24" t="s">
@@ -1429,20 +1478,20 @@
         <v>6</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="44">
+      <c r="J15" s="43">
         <v>0.23369999999999999</v>
       </c>
-      <c r="K15" s="44">
+      <c r="K15" s="43">
         <v>0.45979999999999999</v>
       </c>
-      <c r="L15" s="44">
+      <c r="L15" s="43">
         <v>0.216</v>
       </c>
-      <c r="M15" s="44">
+      <c r="M15" s="43">
         <v>0.40529999999999999</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="54">
+      <c r="O15" s="53">
         <v>5.2</v>
       </c>
       <c r="P15" s="24" t="s">
@@ -1470,20 +1519,20 @@
         <v>6</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="44">
+      <c r="J16" s="43">
         <v>0.24440000000000001</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="43">
         <v>0.4763</v>
       </c>
-      <c r="L16" s="44">
+      <c r="L16" s="43">
         <v>0.23130000000000001</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="43">
         <v>0.44169999999999998</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="54">
+      <c r="O16" s="53">
         <v>7.1</v>
       </c>
       <c r="P16" s="24" t="s">
@@ -1511,20 +1560,20 @@
         <v>6</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="45">
+      <c r="J17" s="44">
         <v>0.2369</v>
       </c>
-      <c r="K17" s="45">
+      <c r="K17" s="44">
         <v>0.46039999999999998</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="44">
         <v>0.2205</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="44">
         <v>0.41849999999999998</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="55">
+      <c r="O17" s="54">
         <v>8.8000000000000007</v>
       </c>
       <c r="P17" s="26" t="s">
@@ -1552,20 +1601,20 @@
         <v>6</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="46">
+      <c r="J18" s="45">
         <v>0.29420000000000002</v>
       </c>
-      <c r="K18" s="46">
+      <c r="K18" s="45">
         <v>0.62180000000000002</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="45">
         <v>0.27579999999999999</v>
       </c>
-      <c r="M18" s="46">
+      <c r="M18" s="45">
         <v>0.59919999999999995</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="56">
+      <c r="O18" s="55">
         <v>1.8</v>
       </c>
       <c r="P18" s="28" t="s">
@@ -1593,20 +1642,20 @@
         <v>6</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="46">
+      <c r="J19" s="45">
         <v>0.2576</v>
       </c>
-      <c r="K19" s="46">
+      <c r="K19" s="45">
         <v>0.50990000000000002</v>
       </c>
-      <c r="L19" s="46">
+      <c r="L19" s="45">
         <v>0.24279999999999999</v>
       </c>
-      <c r="M19" s="46">
+      <c r="M19" s="45">
         <v>0.48770000000000002</v>
       </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="56">
+      <c r="O19" s="55">
         <v>5.2</v>
       </c>
       <c r="P19" s="28" t="s">
@@ -1634,20 +1683,20 @@
         <v>6</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="46">
+      <c r="J20" s="45">
         <v>0.24970000000000001</v>
       </c>
-      <c r="K20" s="46">
+      <c r="K20" s="45">
         <v>0.4894</v>
       </c>
-      <c r="L20" s="46">
+      <c r="L20" s="45">
         <v>0.2356</v>
       </c>
-      <c r="M20" s="46">
+      <c r="M20" s="45">
         <v>0.46839999999999998</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="56">
+      <c r="O20" s="55">
         <v>6.8</v>
       </c>
       <c r="P20" s="28" t="s">
@@ -1675,20 +1724,20 @@
         <v>6</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="46">
+      <c r="J21" s="45">
         <v>0.2462</v>
       </c>
-      <c r="K21" s="46">
+      <c r="K21" s="45">
         <v>0.47820000000000001</v>
       </c>
-      <c r="L21" s="46">
+      <c r="L21" s="45">
         <v>0.2324</v>
       </c>
-      <c r="M21" s="46">
+      <c r="M21" s="45">
         <v>0.46629999999999999</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="56">
+      <c r="O21" s="55">
         <v>8.5</v>
       </c>
       <c r="P21" s="28" t="s">
@@ -1709,7 +1758,7 @@
       <c r="L22" s="33"/>
       <c r="M22" s="33"/>
       <c r="N22" s="33"/>
-      <c r="O22" s="57"/>
+      <c r="O22" s="56"/>
       <c r="P22" s="33"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
@@ -1731,29 +1780,29 @@
         <v>6</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="47">
+      <c r="J23" s="46">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="K23" s="47">
+      <c r="K23" s="46">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="L23" s="47">
+      <c r="L23" s="46">
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="M23" s="47">
+      <c r="M23" s="46">
         <v>0.12939999999999999</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="O23" s="58">
+      <c r="O23" s="57">
         <v>1.8</v>
       </c>
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="62" t="s">
+      <c r="Q23" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="61"/>
+      <c r="R23" s="66"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1774,27 +1823,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="47">
+      <c r="J24" s="46">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="K24" s="47">
+      <c r="K24" s="46">
         <v>8.6E-3</v>
       </c>
-      <c r="L24" s="47">
+      <c r="L24" s="46">
         <v>5.62E-2</v>
       </c>
-      <c r="M24" s="47">
+      <c r="M24" s="46">
         <v>0.1293</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="58">
+      <c r="O24" s="57">
         <v>3.6</v>
       </c>
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="61"/>
+      <c r="Q24" s="67"/>
+      <c r="R24" s="66"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -1815,27 +1864,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="47">
+      <c r="J25" s="46">
         <v>1.4E-3</v>
       </c>
-      <c r="K25" s="47">
+      <c r="K25" s="46">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="46">
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="M25" s="47">
+      <c r="M25" s="46">
         <v>0.1212</v>
       </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="58">
+      <c r="O25" s="57">
         <v>5.4</v>
       </c>
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="61"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="66"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -1856,27 +1905,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="47">
+      <c r="J26" s="46">
         <v>1.8E-3</v>
       </c>
-      <c r="K26" s="47">
+      <c r="K26" s="46">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="L26" s="47">
+      <c r="L26" s="46">
         <v>5.4399999999999997E-2</v>
       </c>
-      <c r="M26" s="47">
+      <c r="M26" s="46">
         <v>0.1237</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="58">
+      <c r="O26" s="57">
         <v>7.2</v>
       </c>
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="61"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="66"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -1897,27 +1946,27 @@
         <v>6</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="47">
+      <c r="J27" s="46">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="K27" s="47">
+      <c r="K27" s="46">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="L27" s="47">
+      <c r="L27" s="46">
         <v>5.62E-2</v>
       </c>
-      <c r="M27" s="47">
+      <c r="M27" s="46">
         <v>0.12820000000000001</v>
       </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="58">
+      <c r="O27" s="57">
         <v>8.9</v>
       </c>
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="61"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="66"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -1938,27 +1987,27 @@
         <v>6</v>
       </c>
       <c r="I28" s="2"/>
-      <c r="J28" s="44">
+      <c r="J28" s="43">
         <v>7.6E-3</v>
       </c>
-      <c r="K28" s="44">
+      <c r="K28" s="43">
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="L28" s="44">
+      <c r="L28" s="43">
         <v>6.1199999999999997E-2</v>
       </c>
-      <c r="M28" s="44">
+      <c r="M28" s="43">
         <v>0.12180000000000001</v>
       </c>
       <c r="N28" s="2"/>
-      <c r="O28" s="54">
+      <c r="O28" s="53">
         <v>1.8</v>
       </c>
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="61"/>
+      <c r="Q28" s="67"/>
+      <c r="R28" s="66"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -1979,27 +2028,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="44">
+      <c r="J29" s="43">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="K29" s="44">
+      <c r="K29" s="43">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="L29" s="44">
+      <c r="L29" s="43">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="M29" s="44">
+      <c r="M29" s="43">
         <v>0.1138</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="O29" s="54">
+      <c r="O29" s="53">
         <v>3.6</v>
       </c>
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="61"/>
+      <c r="Q29" s="67"/>
+      <c r="R29" s="66"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2020,27 +2069,27 @@
         <v>6</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="44">
+      <c r="J30" s="43">
         <v>1.8E-3</v>
       </c>
-      <c r="K30" s="44">
+      <c r="K30" s="43">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="L30" s="44">
+      <c r="L30" s="43">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="M30" s="44">
+      <c r="M30" s="43">
         <v>0.1149</v>
       </c>
       <c r="N30" s="2"/>
-      <c r="O30" s="54">
+      <c r="O30" s="53">
         <v>5.3</v>
       </c>
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="61"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="66"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2061,27 +2110,27 @@
         <v>6</v>
       </c>
       <c r="I31" s="2"/>
-      <c r="J31" s="44">
+      <c r="J31" s="43">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="K31" s="44">
+      <c r="K31" s="43">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="L31" s="44">
+      <c r="L31" s="43">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="M31" s="44">
+      <c r="M31" s="43">
         <v>0.1221</v>
       </c>
       <c r="N31" s="2"/>
-      <c r="O31" s="54">
+      <c r="O31" s="53">
         <v>7</v>
       </c>
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="61"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="66"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2102,27 +2151,27 @@
         <v>6</v>
       </c>
       <c r="I32" s="2"/>
-      <c r="J32" s="44">
+      <c r="J32" s="43">
         <v>9.3041E-4</v>
       </c>
-      <c r="K32" s="44">
+      <c r="K32" s="43">
         <v>2.3E-3</v>
       </c>
-      <c r="L32" s="44">
+      <c r="L32" s="43">
         <v>5.7700000000000001E-2</v>
       </c>
-      <c r="M32" s="44">
+      <c r="M32" s="43">
         <v>0.1167</v>
       </c>
       <c r="N32" s="2"/>
-      <c r="O32" s="54">
+      <c r="O32" s="53">
         <v>8.8000000000000007</v>
       </c>
-      <c r="P32" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="61"/>
+      <c r="P32" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="66"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2143,27 +2192,27 @@
         <v>6</v>
       </c>
       <c r="I33" s="2"/>
-      <c r="J33" s="46">
+      <c r="J33" s="45">
         <v>2.3900000000000001E-2</v>
       </c>
-      <c r="K33" s="46">
+      <c r="K33" s="45">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="L33" s="46">
+      <c r="L33" s="45">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="M33" s="46">
+      <c r="M33" s="45">
         <v>0.16020000000000001</v>
       </c>
       <c r="N33" s="2"/>
-      <c r="O33" s="56">
+      <c r="O33" s="55">
         <v>1.8</v>
       </c>
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="61"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="66"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2184,27 +2233,27 @@
         <v>6</v>
       </c>
       <c r="I34" s="2"/>
-      <c r="J34" s="46">
+      <c r="J34" s="45">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="K34" s="46">
+      <c r="K34" s="45">
         <v>1.78E-2</v>
       </c>
-      <c r="L34" s="46">
+      <c r="L34" s="45">
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="M34" s="46">
+      <c r="M34" s="45">
         <v>0.16550000000000001</v>
       </c>
       <c r="N34" s="2"/>
-      <c r="O34" s="56">
+      <c r="O34" s="55">
         <v>3.5</v>
       </c>
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="61"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="66"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2225,27 +2274,27 @@
         <v>6</v>
       </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="46">
+      <c r="J35" s="45">
         <v>3.3E-3</v>
       </c>
-      <c r="K35" s="46">
+      <c r="K35" s="45">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="L35" s="46">
+      <c r="L35" s="45">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M35" s="46">
+      <c r="M35" s="45">
         <v>0.1643</v>
       </c>
       <c r="N35" s="2"/>
-      <c r="O35" s="56">
+      <c r="O35" s="55">
         <v>5.2</v>
       </c>
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="61"/>
+      <c r="Q35" s="67"/>
+      <c r="R35" s="66"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2266,27 +2315,27 @@
         <v>6</v>
       </c>
       <c r="I36" s="2"/>
-      <c r="J36" s="46">
+      <c r="J36" s="45">
         <v>2E-3</v>
       </c>
-      <c r="K36" s="46">
+      <c r="K36" s="45">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L36" s="46">
+      <c r="L36" s="45">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="M36" s="46">
+      <c r="M36" s="45">
         <v>0.1593</v>
       </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="56">
+      <c r="O36" s="55">
         <v>6.9</v>
       </c>
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="61"/>
+      <c r="Q36" s="67"/>
+      <c r="R36" s="66"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2307,81 +2356,81 @@
         <v>6</v>
       </c>
       <c r="I37" s="2"/>
-      <c r="J37" s="46">
+      <c r="J37" s="45">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="K37" s="46">
+      <c r="K37" s="45">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L37" s="46">
+      <c r="L37" s="45">
         <v>5.8900000000000001E-2</v>
       </c>
-      <c r="M37" s="46">
+      <c r="M37" s="45">
         <v>0.15870000000000001</v>
       </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="56">
+      <c r="O37" s="55">
         <v>8.8000000000000007</v>
       </c>
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="60"/>
-      <c r="R37" s="61"/>
+      <c r="Q37" s="67"/>
+      <c r="R37" s="66"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="68" t="s">
+      <c r="B39" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="64" t="s">
+      <c r="D40" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="64" t="s">
+      <c r="E40" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="64" t="s">
+      <c r="F40" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="64" t="s">
+      <c r="G40" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="64" t="s">
+      <c r="H40" s="59" t="s">
         <v>11</v>
       </c>
       <c r="I40" s="2"/>
-      <c r="J40" s="65" t="s">
+      <c r="J40" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="K40" s="65" t="s">
+      <c r="K40" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="65" t="s">
+      <c r="L40" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="65" t="s">
+      <c r="M40" s="60" t="s">
         <v>10</v>
       </c>
       <c r="N40" s="2"/>
-      <c r="O40" s="66" t="s">
+      <c r="O40" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="P40" s="67" t="s">
+      <c r="P40" s="62" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2404,12 +2453,22 @@
         <v>6</v>
       </c>
       <c r="I41" s="2"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
+      <c r="J41" s="46">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="K41" s="46">
+        <v>1.41E-2</v>
+      </c>
+      <c r="L41" s="46">
+        <v>5.7299999999999997E-2</v>
+      </c>
+      <c r="M41" s="46">
+        <v>0.13070000000000001</v>
+      </c>
       <c r="N41" s="2"/>
-      <c r="O41" s="32"/>
+      <c r="O41" s="57">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="P41" s="34" t="s">
         <v>17</v>
       </c>
@@ -2433,12 +2492,22 @@
         <v>6</v>
       </c>
       <c r="I42" s="2"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
+      <c r="J42" s="46">
+        <v>1.4E-3</v>
+      </c>
+      <c r="K42" s="46">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="L42" s="46">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="M42" s="46">
+        <v>0.1323</v>
+      </c>
       <c r="N42" s="2"/>
-      <c r="O42" s="32"/>
+      <c r="O42" s="57">
+        <v>10</v>
+      </c>
       <c r="P42" s="34" t="s">
         <v>17</v>
       </c>
@@ -2462,12 +2531,22 @@
         <v>6</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
+      <c r="J43" s="46">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="K43" s="46">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="L43" s="46">
+        <v>5.5300000000000002E-2</v>
+      </c>
+      <c r="M43" s="46">
+        <v>0.12529999999999999</v>
+      </c>
       <c r="N43" s="2"/>
-      <c r="O43" s="32"/>
+      <c r="O43" s="57">
+        <v>15</v>
+      </c>
       <c r="P43" s="34" t="s">
         <v>17</v>
       </c>
@@ -2491,44 +2570,264 @@
         <v>6</v>
       </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
+      <c r="J44" s="46">
+        <v>5.2610999999999999E-4</v>
+      </c>
+      <c r="K44" s="46">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="L44" s="46">
+        <v>5.67E-2</v>
+      </c>
+      <c r="M44" s="46">
+        <v>0.129</v>
+      </c>
       <c r="N44" s="2"/>
-      <c r="O44" s="32"/>
+      <c r="O44" s="57">
+        <v>19.899999999999999</v>
+      </c>
       <c r="P44" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="32">
+      <c r="C45" s="70">
         <v>1E-3</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="7">
         <v>500</v>
       </c>
-      <c r="E45" s="32">
+      <c r="E45" s="70">
         <v>4</v>
       </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32" t="s">
+      <c r="F45" s="7"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70" t="s">
         <v>6</v>
       </c>
       <c r="I45" s="2"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
+      <c r="J45" s="75">
+        <v>1.7221000000000001E-4</v>
+      </c>
+      <c r="K45" s="75">
+        <v>4.3927000000000001E-4</v>
+      </c>
+      <c r="L45" s="75">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="M45" s="75">
+        <v>0.12970000000000001</v>
+      </c>
       <c r="N45" s="2"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="34" t="s">
-        <v>17</v>
-      </c>
+      <c r="O45" s="71">
+        <v>24.9</v>
+      </c>
+      <c r="P45" s="72" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="D46" s="8">
+        <v>100</v>
+      </c>
+      <c r="E46" s="23">
+        <v>8</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" s="74"/>
+      <c r="J46" s="43">
+        <v>1.23E-2</v>
+      </c>
+      <c r="K46" s="43">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="L46" s="43">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="M46" s="43">
+        <v>0.1484</v>
+      </c>
+      <c r="N46" s="74"/>
+      <c r="O46" s="23">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P46" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q46" s="73"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="23">
+        <v>1E-4</v>
+      </c>
+      <c r="D47" s="8">
+        <v>200</v>
+      </c>
+      <c r="E47" s="23">
+        <v>8</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" s="74"/>
+      <c r="J47" s="43">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="K47" s="43">
+        <v>4.3E-3</v>
+      </c>
+      <c r="L47" s="43">
+        <v>6.1899999999999997E-2</v>
+      </c>
+      <c r="M47" s="43">
+        <v>0.1241</v>
+      </c>
+      <c r="N47" s="74"/>
+      <c r="O47" s="23">
+        <v>9.9</v>
+      </c>
+      <c r="P47" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q47" s="73"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="23">
+        <v>1E-4</v>
+      </c>
+      <c r="D48" s="8">
+        <v>300</v>
+      </c>
+      <c r="E48" s="23">
+        <v>8</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I48" s="74"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="74"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q48" s="73"/>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="23">
+        <v>1E-4</v>
+      </c>
+      <c r="D49" s="8">
+        <v>400</v>
+      </c>
+      <c r="E49" s="23">
+        <v>8</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49" s="74"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="74"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q49" s="73"/>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="23">
+        <v>1E-4</v>
+      </c>
+      <c r="D50" s="8">
+        <v>500</v>
+      </c>
+      <c r="E50" s="23">
+        <v>8</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" s="74"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="74"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q50" s="73"/>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="76"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J52" s="76"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="76"/>
+      <c r="M52" s="76"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="76"/>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J54" s="76"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="76"/>
+      <c r="M54" s="76"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J55" s="76"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="76"/>
+      <c r="M55" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Testing - hiperparámetros - métricas
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CC0947-99BA-41AB-9DBE-5D6671F4F8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512E55E-4A5F-4B40-930B-EF737F6A3F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="6390" windowWidth="21600" windowHeight="7155" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals" sheetId="1" r:id="rId1"/>
@@ -201,11 +201,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,13 +253,6 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,35 +506,8 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -588,12 +555,28 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,29 +586,39 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,8 +964,8 @@
   </sheetPr>
   <dimension ref="B2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,24 +986,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1078,20 +1071,20 @@
         <v>6</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="38">
+      <c r="J5" s="75">
         <v>0.54179999999999995</v>
       </c>
-      <c r="K5" s="38">
+      <c r="K5" s="75">
         <v>0.73829999999999996</v>
       </c>
-      <c r="L5" s="38">
+      <c r="L5" s="75">
         <v>0.52149999999999996</v>
       </c>
-      <c r="M5" s="38">
+      <c r="M5" s="75">
         <v>0.72629999999999995</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="47">
+      <c r="O5" s="38">
         <v>71.400000000000006</v>
       </c>
       <c r="P5" s="31" t="s">
@@ -1119,12 +1112,12 @@
         <v>6</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="48"/>
+      <c r="O6" s="39"/>
       <c r="P6" s="13" t="s">
         <v>17</v>
       </c>
@@ -1150,20 +1143,20 @@
         <v>6</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="39">
+      <c r="J7" s="69">
         <v>0.2407</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="69">
         <v>0.49049999999999999</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="69">
         <v>0.22650000000000001</v>
       </c>
-      <c r="M7" s="39">
+      <c r="M7" s="69">
         <v>0.44390000000000002</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="48">
+      <c r="O7" s="39">
         <v>3.8</v>
       </c>
       <c r="P7" s="13" t="s">
@@ -1191,20 +1184,20 @@
         <v>18</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="37">
+      <c r="J8" s="70">
         <v>0.23219999999999999</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="70">
         <v>0.45900000000000002</v>
       </c>
-      <c r="L8" s="37">
+      <c r="L8" s="70">
         <v>0.2359</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="70">
         <v>0.46079999999999999</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="49">
+      <c r="O8" s="40">
         <v>3.6</v>
       </c>
       <c r="P8" s="16" t="s">
@@ -1232,20 +1225,20 @@
         <v>6</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="40">
+      <c r="J9" s="71">
         <v>0.2727</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="71">
         <v>0.55230000000000001</v>
       </c>
-      <c r="L9" s="40">
+      <c r="L9" s="71">
         <v>0.26419999999999999</v>
       </c>
-      <c r="M9" s="40">
+      <c r="M9" s="71">
         <v>0.54920000000000002</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="50">
+      <c r="O9" s="41">
         <v>3.5</v>
       </c>
       <c r="P9" s="16" t="s">
@@ -1273,20 +1266,20 @@
         <v>6</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="41">
+      <c r="J10" s="72">
         <v>0.2329</v>
       </c>
-      <c r="K10" s="41">
+      <c r="K10" s="72">
         <v>0.46639999999999998</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="72">
         <v>0.216</v>
       </c>
-      <c r="M10" s="41">
+      <c r="M10" s="72">
         <v>0.42409999999999998</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="51">
+      <c r="O10" s="42">
         <v>1.8</v>
       </c>
       <c r="P10" s="20" t="s">
@@ -1314,20 +1307,20 @@
         <v>6</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="41">
+      <c r="J11" s="72">
         <v>0.21970000000000001</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="72">
         <v>0.42170000000000002</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="72">
         <v>0.20519999999999999</v>
       </c>
-      <c r="M11" s="41">
+      <c r="M11" s="72">
         <v>0.40229999999999999</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="51">
+      <c r="O11" s="42">
         <v>5.5</v>
       </c>
       <c r="P11" s="20" t="s">
@@ -1355,20 +1348,20 @@
         <v>6</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="41">
+      <c r="J12" s="72">
         <v>0.2291</v>
       </c>
-      <c r="K12" s="41">
+      <c r="K12" s="72">
         <v>0.4466</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="72">
         <v>0.21240000000000001</v>
       </c>
-      <c r="M12" s="41">
+      <c r="M12" s="72">
         <v>0.41060000000000002</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="51">
+      <c r="O12" s="42">
         <v>7.2</v>
       </c>
       <c r="P12" s="20" t="s">
@@ -1396,20 +1389,20 @@
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="42">
+      <c r="J13" s="73">
         <v>0.22589999999999999</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="73">
         <v>0.45029999999999998</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="73">
         <v>0.20860000000000001</v>
       </c>
-      <c r="M13" s="42">
+      <c r="M13" s="73">
         <v>0.4037</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="52">
+      <c r="O13" s="43">
         <v>9.3000000000000007</v>
       </c>
       <c r="P13" s="20" t="s">
@@ -1437,20 +1430,20 @@
         <v>6</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="43">
+      <c r="J14" s="67">
         <v>0.22900000000000001</v>
       </c>
-      <c r="K14" s="43">
+      <c r="K14" s="67">
         <v>0.44979999999999998</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L14" s="67">
         <v>0.2132</v>
       </c>
-      <c r="M14" s="43">
+      <c r="M14" s="67">
         <v>0.40060000000000001</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="53">
+      <c r="O14" s="44">
         <v>1.7</v>
       </c>
       <c r="P14" s="24" t="s">
@@ -1478,20 +1471,20 @@
         <v>6</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="43">
+      <c r="J15" s="67">
         <v>0.23369999999999999</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="67">
         <v>0.45979999999999999</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L15" s="67">
         <v>0.216</v>
       </c>
-      <c r="M15" s="43">
+      <c r="M15" s="67">
         <v>0.40529999999999999</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="53">
+      <c r="O15" s="44">
         <v>5.2</v>
       </c>
       <c r="P15" s="24" t="s">
@@ -1519,20 +1512,20 @@
         <v>6</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="43">
+      <c r="J16" s="67">
         <v>0.24440000000000001</v>
       </c>
-      <c r="K16" s="43">
+      <c r="K16" s="67">
         <v>0.4763</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L16" s="67">
         <v>0.23130000000000001</v>
       </c>
-      <c r="M16" s="43">
+      <c r="M16" s="67">
         <v>0.44169999999999998</v>
       </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="53">
+      <c r="O16" s="44">
         <v>7.1</v>
       </c>
       <c r="P16" s="24" t="s">
@@ -1560,20 +1553,20 @@
         <v>6</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="44">
+      <c r="J17" s="74">
         <v>0.2369</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="74">
         <v>0.46039999999999998</v>
       </c>
-      <c r="L17" s="44">
+      <c r="L17" s="74">
         <v>0.2205</v>
       </c>
-      <c r="M17" s="44">
+      <c r="M17" s="74">
         <v>0.41849999999999998</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="54">
+      <c r="O17" s="45">
         <v>8.8000000000000007</v>
       </c>
       <c r="P17" s="26" t="s">
@@ -1601,20 +1594,20 @@
         <v>6</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="45">
+      <c r="J18" s="68">
         <v>0.29420000000000002</v>
       </c>
-      <c r="K18" s="45">
+      <c r="K18" s="68">
         <v>0.62180000000000002</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="68">
         <v>0.27579999999999999</v>
       </c>
-      <c r="M18" s="45">
+      <c r="M18" s="68">
         <v>0.59919999999999995</v>
       </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="55">
+      <c r="O18" s="46">
         <v>1.8</v>
       </c>
       <c r="P18" s="28" t="s">
@@ -1642,20 +1635,20 @@
         <v>6</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="45">
+      <c r="J19" s="68">
         <v>0.2576</v>
       </c>
-      <c r="K19" s="45">
+      <c r="K19" s="68">
         <v>0.50990000000000002</v>
       </c>
-      <c r="L19" s="45">
+      <c r="L19" s="68">
         <v>0.24279999999999999</v>
       </c>
-      <c r="M19" s="45">
+      <c r="M19" s="68">
         <v>0.48770000000000002</v>
       </c>
       <c r="N19" s="2"/>
-      <c r="O19" s="55">
+      <c r="O19" s="46">
         <v>5.2</v>
       </c>
       <c r="P19" s="28" t="s">
@@ -1683,20 +1676,20 @@
         <v>6</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="45">
+      <c r="J20" s="68">
         <v>0.24970000000000001</v>
       </c>
-      <c r="K20" s="45">
+      <c r="K20" s="68">
         <v>0.4894</v>
       </c>
-      <c r="L20" s="45">
+      <c r="L20" s="68">
         <v>0.2356</v>
       </c>
-      <c r="M20" s="45">
+      <c r="M20" s="68">
         <v>0.46839999999999998</v>
       </c>
       <c r="N20" s="2"/>
-      <c r="O20" s="55">
+      <c r="O20" s="46">
         <v>6.8</v>
       </c>
       <c r="P20" s="28" t="s">
@@ -1724,20 +1717,20 @@
         <v>6</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="45">
+      <c r="J21" s="68">
         <v>0.2462</v>
       </c>
-      <c r="K21" s="45">
+      <c r="K21" s="68">
         <v>0.47820000000000001</v>
       </c>
-      <c r="L21" s="45">
+      <c r="L21" s="68">
         <v>0.2324</v>
       </c>
-      <c r="M21" s="45">
+      <c r="M21" s="68">
         <v>0.46629999999999999</v>
       </c>
       <c r="N21" s="2"/>
-      <c r="O21" s="55">
+      <c r="O21" s="46">
         <v>8.5</v>
       </c>
       <c r="P21" s="28" t="s">
@@ -1758,7 +1751,7 @@
       <c r="L22" s="33"/>
       <c r="M22" s="33"/>
       <c r="N22" s="33"/>
-      <c r="O22" s="56"/>
+      <c r="O22" s="47"/>
       <c r="P22" s="33"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
@@ -1780,29 +1773,29 @@
         <v>6</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="46">
+      <c r="J23" s="65">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="K23" s="46">
+      <c r="K23" s="65">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="L23" s="46">
+      <c r="L23" s="65">
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="M23" s="46">
+      <c r="M23" s="65">
         <v>0.12939999999999999</v>
       </c>
       <c r="N23" s="2"/>
-      <c r="O23" s="57">
+      <c r="O23" s="48">
         <v>1.8</v>
       </c>
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="65" t="s">
+      <c r="Q23" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="66"/>
+      <c r="R23" s="63"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1823,27 +1816,27 @@
         <v>6</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="46">
+      <c r="J24" s="65">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="K24" s="46">
+      <c r="K24" s="65">
         <v>8.6E-3</v>
       </c>
-      <c r="L24" s="46">
+      <c r="L24" s="65">
         <v>5.62E-2</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="65">
         <v>0.1293</v>
       </c>
       <c r="N24" s="2"/>
-      <c r="O24" s="57">
+      <c r="O24" s="48">
         <v>3.6</v>
       </c>
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="66"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="63"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -1864,27 +1857,27 @@
         <v>6</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="46">
+      <c r="J25" s="65">
         <v>1.4E-3</v>
       </c>
-      <c r="K25" s="46">
+      <c r="K25" s="65">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L25" s="46">
+      <c r="L25" s="65">
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="M25" s="46">
+      <c r="M25" s="65">
         <v>0.1212</v>
       </c>
       <c r="N25" s="2"/>
-      <c r="O25" s="57">
+      <c r="O25" s="48">
         <v>5.4</v>
       </c>
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="66"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="63"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -1905,27 +1898,27 @@
         <v>6</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="46">
+      <c r="J26" s="65">
         <v>1.8E-3</v>
       </c>
-      <c r="K26" s="46">
+      <c r="K26" s="65">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="L26" s="46">
+      <c r="L26" s="65">
         <v>5.4399999999999997E-2</v>
       </c>
-      <c r="M26" s="46">
+      <c r="M26" s="65">
         <v>0.1237</v>
       </c>
       <c r="N26" s="2"/>
-      <c r="O26" s="57">
+      <c r="O26" s="48">
         <v>7.2</v>
       </c>
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="67"/>
-      <c r="R26" s="66"/>
+      <c r="Q26" s="64"/>
+      <c r="R26" s="63"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -1946,27 +1939,27 @@
         <v>6</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="46">
+      <c r="J27" s="65">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="K27" s="46">
+      <c r="K27" s="65">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="L27" s="46">
+      <c r="L27" s="65">
         <v>5.62E-2</v>
       </c>
-      <c r="M27" s="46">
+      <c r="M27" s="65">
         <v>0.12820000000000001</v>
       </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="57">
+      <c r="O27" s="48">
         <v>8.9</v>
       </c>
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="67"/>
-      <c r="R27" s="66"/>
+      <c r="Q27" s="64"/>
+      <c r="R27" s="63"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -1987,27 +1980,27 @@
         <v>6</v>
       </c>
       <c r="I28" s="2"/>
-      <c r="J28" s="43">
+      <c r="J28" s="67">
         <v>7.6E-3</v>
       </c>
-      <c r="K28" s="43">
+      <c r="K28" s="67">
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="L28" s="43">
+      <c r="L28" s="67">
         <v>6.1199999999999997E-2</v>
       </c>
-      <c r="M28" s="43">
+      <c r="M28" s="67">
         <v>0.12180000000000001</v>
       </c>
       <c r="N28" s="2"/>
-      <c r="O28" s="53">
+      <c r="O28" s="44">
         <v>1.8</v>
       </c>
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="67"/>
-      <c r="R28" s="66"/>
+      <c r="Q28" s="64"/>
+      <c r="R28" s="63"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2028,27 +2021,27 @@
         <v>6</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="43">
+      <c r="J29" s="67">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="K29" s="43">
+      <c r="K29" s="67">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="L29" s="43">
+      <c r="L29" s="67">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="M29" s="43">
+      <c r="M29" s="67">
         <v>0.1138</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="O29" s="53">
+      <c r="O29" s="44">
         <v>3.6</v>
       </c>
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="67"/>
-      <c r="R29" s="66"/>
+      <c r="Q29" s="64"/>
+      <c r="R29" s="63"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2069,27 +2062,27 @@
         <v>6</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="43">
+      <c r="J30" s="67">
         <v>1.8E-3</v>
       </c>
-      <c r="K30" s="43">
+      <c r="K30" s="67">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="L30" s="43">
+      <c r="L30" s="67">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="M30" s="43">
+      <c r="M30" s="67">
         <v>0.1149</v>
       </c>
       <c r="N30" s="2"/>
-      <c r="O30" s="53">
+      <c r="O30" s="44">
         <v>5.3</v>
       </c>
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="67"/>
-      <c r="R30" s="66"/>
+      <c r="Q30" s="64"/>
+      <c r="R30" s="63"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2110,27 +2103,27 @@
         <v>6</v>
       </c>
       <c r="I31" s="2"/>
-      <c r="J31" s="43">
+      <c r="J31" s="67">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="K31" s="43">
+      <c r="K31" s="67">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="L31" s="43">
+      <c r="L31" s="67">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="M31" s="43">
+      <c r="M31" s="67">
         <v>0.1221</v>
       </c>
       <c r="N31" s="2"/>
-      <c r="O31" s="53">
+      <c r="O31" s="44">
         <v>7</v>
       </c>
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="66"/>
+      <c r="Q31" s="64"/>
+      <c r="R31" s="63"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2151,27 +2144,27 @@
         <v>6</v>
       </c>
       <c r="I32" s="2"/>
-      <c r="J32" s="43">
+      <c r="J32" s="67">
         <v>9.3041E-4</v>
       </c>
-      <c r="K32" s="43">
+      <c r="K32" s="67">
         <v>2.3E-3</v>
       </c>
-      <c r="L32" s="43">
+      <c r="L32" s="67">
         <v>5.7700000000000001E-2</v>
       </c>
-      <c r="M32" s="43">
+      <c r="M32" s="67">
         <v>0.1167</v>
       </c>
       <c r="N32" s="2"/>
-      <c r="O32" s="53">
+      <c r="O32" s="44">
         <v>8.8000000000000007</v>
       </c>
-      <c r="P32" s="68" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q32" s="67"/>
-      <c r="R32" s="66"/>
+      <c r="P32" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q32" s="64"/>
+      <c r="R32" s="63"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2192,27 +2185,27 @@
         <v>6</v>
       </c>
       <c r="I33" s="2"/>
-      <c r="J33" s="45">
+      <c r="J33" s="68">
         <v>2.3900000000000001E-2</v>
       </c>
-      <c r="K33" s="45">
+      <c r="K33" s="68">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="L33" s="45">
+      <c r="L33" s="68">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="M33" s="45">
+      <c r="M33" s="68">
         <v>0.16020000000000001</v>
       </c>
       <c r="N33" s="2"/>
-      <c r="O33" s="55">
+      <c r="O33" s="46">
         <v>1.8</v>
       </c>
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="67"/>
-      <c r="R33" s="66"/>
+      <c r="Q33" s="64"/>
+      <c r="R33" s="63"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2233,27 +2226,27 @@
         <v>6</v>
       </c>
       <c r="I34" s="2"/>
-      <c r="J34" s="45">
+      <c r="J34" s="68">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="K34" s="45">
+      <c r="K34" s="68">
         <v>1.78E-2</v>
       </c>
-      <c r="L34" s="45">
+      <c r="L34" s="68">
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="M34" s="45">
+      <c r="M34" s="68">
         <v>0.16550000000000001</v>
       </c>
       <c r="N34" s="2"/>
-      <c r="O34" s="55">
+      <c r="O34" s="46">
         <v>3.5</v>
       </c>
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="67"/>
-      <c r="R34" s="66"/>
+      <c r="Q34" s="64"/>
+      <c r="R34" s="63"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2274,27 +2267,27 @@
         <v>6</v>
       </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="45">
+      <c r="J35" s="68">
         <v>3.3E-3</v>
       </c>
-      <c r="K35" s="45">
+      <c r="K35" s="68">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="L35" s="45">
+      <c r="L35" s="68">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M35" s="45">
+      <c r="M35" s="68">
         <v>0.1643</v>
       </c>
       <c r="N35" s="2"/>
-      <c r="O35" s="55">
+      <c r="O35" s="46">
         <v>5.2</v>
       </c>
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="67"/>
-      <c r="R35" s="66"/>
+      <c r="Q35" s="64"/>
+      <c r="R35" s="63"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2315,27 +2308,27 @@
         <v>6</v>
       </c>
       <c r="I36" s="2"/>
-      <c r="J36" s="45">
+      <c r="J36" s="68">
         <v>2E-3</v>
       </c>
-      <c r="K36" s="45">
+      <c r="K36" s="68">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L36" s="45">
+      <c r="L36" s="68">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="M36" s="45">
+      <c r="M36" s="68">
         <v>0.1593</v>
       </c>
       <c r="N36" s="2"/>
-      <c r="O36" s="55">
+      <c r="O36" s="46">
         <v>6.9</v>
       </c>
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="67"/>
-      <c r="R36" s="66"/>
+      <c r="Q36" s="64"/>
+      <c r="R36" s="63"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2356,81 +2349,81 @@
         <v>6</v>
       </c>
       <c r="I37" s="2"/>
-      <c r="J37" s="45">
+      <c r="J37" s="68">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="K37" s="45">
+      <c r="K37" s="68">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L37" s="45">
+      <c r="L37" s="68">
         <v>5.8900000000000001E-2</v>
       </c>
-      <c r="M37" s="45">
+      <c r="M37" s="68">
         <v>0.15870000000000001</v>
       </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="55">
+      <c r="O37" s="46">
         <v>8.8000000000000007</v>
       </c>
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="67"/>
-      <c r="R37" s="66"/>
+      <c r="Q37" s="64"/>
+      <c r="R37" s="63"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="69"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="59" t="s">
+      <c r="E40" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="59" t="s">
+      <c r="F40" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="59" t="s">
+      <c r="G40" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="59" t="s">
+      <c r="H40" s="50" t="s">
         <v>11</v>
       </c>
       <c r="I40" s="2"/>
-      <c r="J40" s="60" t="s">
+      <c r="J40" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K40" s="60" t="s">
+      <c r="K40" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="L40" s="60" t="s">
+      <c r="L40" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="60" t="s">
+      <c r="M40" s="51" t="s">
         <v>10</v>
       </c>
       <c r="N40" s="2"/>
-      <c r="O40" s="61" t="s">
+      <c r="O40" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="P40" s="62" t="s">
+      <c r="P40" s="53" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2439,7 +2432,7 @@
         <v>43</v>
       </c>
       <c r="C41" s="32">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D41" s="6">
         <v>100</v>
@@ -2453,20 +2446,20 @@
         <v>6</v>
       </c>
       <c r="I41" s="2"/>
-      <c r="J41" s="46">
+      <c r="J41" s="65">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="K41" s="46">
+      <c r="K41" s="65">
         <v>1.41E-2</v>
       </c>
-      <c r="L41" s="46">
+      <c r="L41" s="65">
         <v>5.7299999999999997E-2</v>
       </c>
-      <c r="M41" s="46">
+      <c r="M41" s="65">
         <v>0.13070000000000001</v>
       </c>
       <c r="N41" s="2"/>
-      <c r="O41" s="57">
+      <c r="O41" s="48">
         <v>5.0999999999999996</v>
       </c>
       <c r="P41" s="34" t="s">
@@ -2478,7 +2471,7 @@
         <v>44</v>
       </c>
       <c r="C42" s="32">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D42" s="6">
         <v>200</v>
@@ -2492,20 +2485,20 @@
         <v>6</v>
       </c>
       <c r="I42" s="2"/>
-      <c r="J42" s="46">
+      <c r="J42" s="65">
         <v>1.4E-3</v>
       </c>
-      <c r="K42" s="46">
+      <c r="K42" s="65">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L42" s="46">
+      <c r="L42" s="65">
         <v>5.8099999999999999E-2</v>
       </c>
-      <c r="M42" s="46">
+      <c r="M42" s="65">
         <v>0.1323</v>
       </c>
       <c r="N42" s="2"/>
-      <c r="O42" s="57">
+      <c r="O42" s="48">
         <v>10</v>
       </c>
       <c r="P42" s="34" t="s">
@@ -2517,7 +2510,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="32">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D43" s="6">
         <v>300</v>
@@ -2531,20 +2524,20 @@
         <v>6</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="46">
+      <c r="J43" s="65">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="K43" s="46">
+      <c r="K43" s="65">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="L43" s="46">
+      <c r="L43" s="65">
         <v>5.5300000000000002E-2</v>
       </c>
-      <c r="M43" s="46">
+      <c r="M43" s="65">
         <v>0.12529999999999999</v>
       </c>
       <c r="N43" s="2"/>
-      <c r="O43" s="57">
+      <c r="O43" s="48">
         <v>15</v>
       </c>
       <c r="P43" s="34" t="s">
@@ -2556,7 +2549,7 @@
         <v>46</v>
       </c>
       <c r="C44" s="32">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D44" s="6">
         <v>400</v>
@@ -2570,20 +2563,20 @@
         <v>6</v>
       </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="46">
+      <c r="J44" s="65">
         <v>5.2610999999999999E-4</v>
       </c>
-      <c r="K44" s="46">
+      <c r="K44" s="65">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="L44" s="46">
+      <c r="L44" s="65">
         <v>5.67E-2</v>
       </c>
-      <c r="M44" s="46">
+      <c r="M44" s="65">
         <v>0.129</v>
       </c>
       <c r="N44" s="2"/>
-      <c r="O44" s="57">
+      <c r="O44" s="48">
         <v>19.899999999999999</v>
       </c>
       <c r="P44" s="34" t="s">
@@ -2594,38 +2587,38 @@
       <c r="B45" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="70">
-        <v>1E-3</v>
+      <c r="C45" s="54">
+        <v>1E-4</v>
       </c>
       <c r="D45" s="7">
         <v>500</v>
       </c>
-      <c r="E45" s="70">
+      <c r="E45" s="54">
         <v>4</v>
       </c>
       <c r="F45" s="7"/>
-      <c r="G45" s="70"/>
-      <c r="H45" s="70" t="s">
+      <c r="G45" s="54"/>
+      <c r="H45" s="54" t="s">
         <v>6</v>
       </c>
       <c r="I45" s="2"/>
-      <c r="J45" s="75">
+      <c r="J45" s="66">
         <v>1.7221000000000001E-4</v>
       </c>
-      <c r="K45" s="75">
+      <c r="K45" s="66">
         <v>4.3927000000000001E-4</v>
       </c>
-      <c r="L45" s="75">
+      <c r="L45" s="66">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="M45" s="75">
+      <c r="M45" s="66">
         <v>0.12970000000000001</v>
       </c>
       <c r="N45" s="2"/>
-      <c r="O45" s="71">
+      <c r="O45" s="55">
         <v>24.9</v>
       </c>
-      <c r="P45" s="72" t="s">
+      <c r="P45" s="56" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2634,7 +2627,7 @@
         <v>48</v>
       </c>
       <c r="C46" s="23">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="D46" s="8">
         <v>100</v>
@@ -2647,27 +2640,26 @@
       <c r="H46" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I46" s="74"/>
-      <c r="J46" s="43">
+      <c r="I46" s="57"/>
+      <c r="J46" s="67">
         <v>1.23E-2</v>
       </c>
-      <c r="K46" s="43">
+      <c r="K46" s="67">
         <v>3.1300000000000001E-2</v>
       </c>
-      <c r="L46" s="43">
+      <c r="L46" s="67">
         <v>7.0499999999999993E-2</v>
       </c>
-      <c r="M46" s="43">
+      <c r="M46" s="67">
         <v>0.1484</v>
       </c>
-      <c r="N46" s="74"/>
+      <c r="N46" s="57"/>
       <c r="O46" s="23">
         <v>5.0999999999999996</v>
       </c>
       <c r="P46" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q46" s="73"/>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
@@ -2687,27 +2679,26 @@
       <c r="H47" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I47" s="74"/>
-      <c r="J47" s="43">
+      <c r="I47" s="57"/>
+      <c r="J47" s="67">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="K47" s="43">
+      <c r="K47" s="67">
         <v>4.3E-3</v>
       </c>
-      <c r="L47" s="43">
+      <c r="L47" s="67">
         <v>6.1899999999999997E-2</v>
       </c>
-      <c r="M47" s="43">
+      <c r="M47" s="67">
         <v>0.1241</v>
       </c>
-      <c r="N47" s="74"/>
+      <c r="N47" s="57"/>
       <c r="O47" s="23">
         <v>9.9</v>
       </c>
       <c r="P47" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q47" s="73"/>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="18" t="s">
@@ -2727,19 +2718,28 @@
       <c r="H48" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I48" s="74"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="43"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="23"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="67">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K48" s="67">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="L48" s="67">
+        <v>6.2799999999999995E-2</v>
+      </c>
+      <c r="M48" s="67">
+        <v>0.1278</v>
+      </c>
+      <c r="N48" s="57"/>
+      <c r="O48" s="23">
+        <v>14.8</v>
+      </c>
       <c r="P48" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q48" s="73"/>
-    </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>51</v>
       </c>
@@ -2757,19 +2757,28 @@
       <c r="H49" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I49" s="74"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="74"/>
-      <c r="O49" s="23"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="67">
+        <v>8.6755000000000003E-4</v>
+      </c>
+      <c r="K49" s="67">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="L49" s="67">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="M49" s="67">
+        <v>0.13569999999999999</v>
+      </c>
+      <c r="N49" s="57"/>
+      <c r="O49" s="23">
+        <v>19.600000000000001</v>
+      </c>
       <c r="P49" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q49" s="73"/>
-    </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>52</v>
       </c>
@@ -2787,47 +2796,56 @@
       <c r="H50" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I50" s="74"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-      <c r="M50" s="43"/>
-      <c r="N50" s="74"/>
-      <c r="O50" s="23"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="67">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K50" s="67">
+        <v>2.8E-3</v>
+      </c>
+      <c r="L50" s="67">
+        <v>6.3700000000000007E-2</v>
+      </c>
+      <c r="M50" s="67">
+        <v>0.1268</v>
+      </c>
+      <c r="N50" s="57"/>
+      <c r="O50" s="23">
+        <v>24.5</v>
+      </c>
       <c r="P50" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q50" s="73"/>
-    </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J51" s="76"/>
-      <c r="K51" s="76"/>
-      <c r="L51" s="76"/>
-      <c r="M51" s="76"/>
-    </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J52" s="76"/>
-      <c r="K52" s="76"/>
-      <c r="L52" s="76"/>
-      <c r="M52" s="76"/>
-    </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J53" s="76"/>
-      <c r="K53" s="76"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="76"/>
-    </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J54" s="76"/>
-      <c r="K54" s="76"/>
-      <c r="L54" s="76"/>
-      <c r="M54" s="76"/>
-    </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J55" s="76"/>
-      <c r="K55" s="76"/>
-      <c r="L55" s="76"/>
-      <c r="M55" s="76"/>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J51" s="58"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="58"/>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J52" s="58"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J53" s="58"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J54" s="58"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J55" s="58"/>
+      <c r="K55" s="58"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Add & Testing - aplicación cosine decay y análisis de métricas
Por ahora se puede ver que se pouede obtener un error más bajo en comparación a los modelos anteriores, pero la cantidad de epocas son muchas, Se aumentará el número de inputs si el error NMSE luego de calcular la ICWT es alto.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512E55E-4A5F-4B40-930B-EF737F6A3F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25135F7-4796-4D64-BC2A-652C6C0B1207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
-    <sheet name="full_signals" sheetId="1" r:id="rId1"/>
+    <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
+    <sheet name="full_signals - with decay" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="61">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -195,16 +196,39 @@
   </si>
   <si>
     <t>modelo 32</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>model/hip</t>
+  </si>
+  <si>
+    <t>max_epoch</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>warm_steps(20%)</t>
+  </si>
+  <si>
+    <t>decay_steps (80%)</t>
+  </si>
+  <si>
+    <t>tiempo de entrenamiento (min)</t>
+  </si>
+  <si>
+    <t># inputs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -265,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,8 +374,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -396,11 +426,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,6 +622,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,37 +670,25 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -962,10 +1034,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B2:R55"/>
+  <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,24 +1058,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1071,16 +1143,16 @@
         <v>6</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="75">
+      <c r="J5" s="68">
         <v>0.54179999999999995</v>
       </c>
-      <c r="K5" s="75">
+      <c r="K5" s="68">
         <v>0.73829999999999996</v>
       </c>
-      <c r="L5" s="75">
+      <c r="L5" s="68">
         <v>0.52149999999999996</v>
       </c>
-      <c r="M5" s="75">
+      <c r="M5" s="68">
         <v>0.72629999999999995</v>
       </c>
       <c r="N5" s="2"/>
@@ -1143,16 +1215,16 @@
         <v>6</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="69">
+      <c r="J7" s="37">
         <v>0.2407</v>
       </c>
-      <c r="K7" s="69">
+      <c r="K7" s="37">
         <v>0.49049999999999999</v>
       </c>
-      <c r="L7" s="69">
+      <c r="L7" s="37">
         <v>0.22650000000000001</v>
       </c>
-      <c r="M7" s="69">
+      <c r="M7" s="37">
         <v>0.44390000000000002</v>
       </c>
       <c r="N7" s="2"/>
@@ -1184,16 +1256,16 @@
         <v>18</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="70">
+      <c r="J8" s="63">
         <v>0.23219999999999999</v>
       </c>
-      <c r="K8" s="70">
+      <c r="K8" s="63">
         <v>0.45900000000000002</v>
       </c>
-      <c r="L8" s="70">
+      <c r="L8" s="63">
         <v>0.2359</v>
       </c>
-      <c r="M8" s="70">
+      <c r="M8" s="63">
         <v>0.46079999999999999</v>
       </c>
       <c r="N8" s="2"/>
@@ -1225,16 +1297,16 @@
         <v>6</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="71">
+      <c r="J9" s="64">
         <v>0.2727</v>
       </c>
-      <c r="K9" s="71">
+      <c r="K9" s="64">
         <v>0.55230000000000001</v>
       </c>
-      <c r="L9" s="71">
+      <c r="L9" s="64">
         <v>0.26419999999999999</v>
       </c>
-      <c r="M9" s="71">
+      <c r="M9" s="64">
         <v>0.54920000000000002</v>
       </c>
       <c r="N9" s="2"/>
@@ -1266,16 +1338,16 @@
         <v>6</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="72">
+      <c r="J10" s="65">
         <v>0.2329</v>
       </c>
-      <c r="K10" s="72">
+      <c r="K10" s="65">
         <v>0.46639999999999998</v>
       </c>
-      <c r="L10" s="72">
+      <c r="L10" s="65">
         <v>0.216</v>
       </c>
-      <c r="M10" s="72">
+      <c r="M10" s="65">
         <v>0.42409999999999998</v>
       </c>
       <c r="N10" s="2"/>
@@ -1307,16 +1379,16 @@
         <v>6</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="72">
+      <c r="J11" s="65">
         <v>0.21970000000000001</v>
       </c>
-      <c r="K11" s="72">
+      <c r="K11" s="65">
         <v>0.42170000000000002</v>
       </c>
-      <c r="L11" s="72">
+      <c r="L11" s="65">
         <v>0.20519999999999999</v>
       </c>
-      <c r="M11" s="72">
+      <c r="M11" s="65">
         <v>0.40229999999999999</v>
       </c>
       <c r="N11" s="2"/>
@@ -1348,16 +1420,16 @@
         <v>6</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="72">
+      <c r="J12" s="65">
         <v>0.2291</v>
       </c>
-      <c r="K12" s="72">
+      <c r="K12" s="65">
         <v>0.4466</v>
       </c>
-      <c r="L12" s="72">
+      <c r="L12" s="65">
         <v>0.21240000000000001</v>
       </c>
-      <c r="M12" s="72">
+      <c r="M12" s="65">
         <v>0.41060000000000002</v>
       </c>
       <c r="N12" s="2"/>
@@ -1389,16 +1461,16 @@
         <v>6</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="73">
+      <c r="J13" s="66">
         <v>0.22589999999999999</v>
       </c>
-      <c r="K13" s="73">
+      <c r="K13" s="66">
         <v>0.45029999999999998</v>
       </c>
-      <c r="L13" s="73">
+      <c r="L13" s="66">
         <v>0.20860000000000001</v>
       </c>
-      <c r="M13" s="73">
+      <c r="M13" s="66">
         <v>0.4037</v>
       </c>
       <c r="N13" s="2"/>
@@ -1430,16 +1502,16 @@
         <v>6</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="67">
+      <c r="J14" s="60">
         <v>0.22900000000000001</v>
       </c>
-      <c r="K14" s="67">
+      <c r="K14" s="60">
         <v>0.44979999999999998</v>
       </c>
-      <c r="L14" s="67">
+      <c r="L14" s="60">
         <v>0.2132</v>
       </c>
-      <c r="M14" s="67">
+      <c r="M14" s="60">
         <v>0.40060000000000001</v>
       </c>
       <c r="N14" s="2"/>
@@ -1471,16 +1543,16 @@
         <v>6</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="67">
+      <c r="J15" s="60">
         <v>0.23369999999999999</v>
       </c>
-      <c r="K15" s="67">
+      <c r="K15" s="60">
         <v>0.45979999999999999</v>
       </c>
-      <c r="L15" s="67">
+      <c r="L15" s="60">
         <v>0.216</v>
       </c>
-      <c r="M15" s="67">
+      <c r="M15" s="60">
         <v>0.40529999999999999</v>
       </c>
       <c r="N15" s="2"/>
@@ -1512,16 +1584,16 @@
         <v>6</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="67">
+      <c r="J16" s="60">
         <v>0.24440000000000001</v>
       </c>
-      <c r="K16" s="67">
+      <c r="K16" s="60">
         <v>0.4763</v>
       </c>
-      <c r="L16" s="67">
+      <c r="L16" s="60">
         <v>0.23130000000000001</v>
       </c>
-      <c r="M16" s="67">
+      <c r="M16" s="60">
         <v>0.44169999999999998</v>
       </c>
       <c r="N16" s="2"/>
@@ -1553,16 +1625,16 @@
         <v>6</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="74">
+      <c r="J17" s="67">
         <v>0.2369</v>
       </c>
-      <c r="K17" s="74">
+      <c r="K17" s="67">
         <v>0.46039999999999998</v>
       </c>
-      <c r="L17" s="74">
+      <c r="L17" s="67">
         <v>0.2205</v>
       </c>
-      <c r="M17" s="74">
+      <c r="M17" s="67">
         <v>0.41849999999999998</v>
       </c>
       <c r="N17" s="2"/>
@@ -1594,16 +1666,16 @@
         <v>6</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="68">
+      <c r="J18" s="61">
         <v>0.29420000000000002</v>
       </c>
-      <c r="K18" s="68">
+      <c r="K18" s="61">
         <v>0.62180000000000002</v>
       </c>
-      <c r="L18" s="68">
+      <c r="L18" s="61">
         <v>0.27579999999999999</v>
       </c>
-      <c r="M18" s="68">
+      <c r="M18" s="61">
         <v>0.59919999999999995</v>
       </c>
       <c r="N18" s="2"/>
@@ -1635,16 +1707,16 @@
         <v>6</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="68">
+      <c r="J19" s="61">
         <v>0.2576</v>
       </c>
-      <c r="K19" s="68">
+      <c r="K19" s="61">
         <v>0.50990000000000002</v>
       </c>
-      <c r="L19" s="68">
+      <c r="L19" s="61">
         <v>0.24279999999999999</v>
       </c>
-      <c r="M19" s="68">
+      <c r="M19" s="61">
         <v>0.48770000000000002</v>
       </c>
       <c r="N19" s="2"/>
@@ -1676,16 +1748,16 @@
         <v>6</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="68">
+      <c r="J20" s="61">
         <v>0.24970000000000001</v>
       </c>
-      <c r="K20" s="68">
+      <c r="K20" s="61">
         <v>0.4894</v>
       </c>
-      <c r="L20" s="68">
+      <c r="L20" s="61">
         <v>0.2356</v>
       </c>
-      <c r="M20" s="68">
+      <c r="M20" s="61">
         <v>0.46839999999999998</v>
       </c>
       <c r="N20" s="2"/>
@@ -1717,16 +1789,16 @@
         <v>6</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="68">
+      <c r="J21" s="61">
         <v>0.2462</v>
       </c>
-      <c r="K21" s="68">
+      <c r="K21" s="61">
         <v>0.47820000000000001</v>
       </c>
-      <c r="L21" s="68">
+      <c r="L21" s="61">
         <v>0.2324</v>
       </c>
-      <c r="M21" s="68">
+      <c r="M21" s="61">
         <v>0.46629999999999999</v>
       </c>
       <c r="N21" s="2"/>
@@ -1773,16 +1845,16 @@
         <v>6</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="65">
+      <c r="J23" s="59">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="K23" s="65">
+      <c r="K23" s="59">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="L23" s="65">
+      <c r="L23" s="59">
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="M23" s="65">
+      <c r="M23" s="59">
         <v>0.12939999999999999</v>
       </c>
       <c r="N23" s="2"/>
@@ -1792,10 +1864,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="62" t="s">
+      <c r="Q23" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="63"/>
+      <c r="R23" s="73"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1816,16 +1888,16 @@
         <v>6</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="65">
+      <c r="J24" s="59">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="K24" s="65">
+      <c r="K24" s="59">
         <v>8.6E-3</v>
       </c>
-      <c r="L24" s="65">
+      <c r="L24" s="59">
         <v>5.62E-2</v>
       </c>
-      <c r="M24" s="65">
+      <c r="M24" s="59">
         <v>0.1293</v>
       </c>
       <c r="N24" s="2"/>
@@ -1835,8 +1907,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="63"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="73"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -1857,16 +1929,16 @@
         <v>6</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="65">
+      <c r="J25" s="59">
         <v>1.4E-3</v>
       </c>
-      <c r="K25" s="65">
+      <c r="K25" s="59">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L25" s="65">
+      <c r="L25" s="59">
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="M25" s="65">
+      <c r="M25" s="59">
         <v>0.1212</v>
       </c>
       <c r="N25" s="2"/>
@@ -1876,8 +1948,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="63"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="73"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -1898,16 +1970,16 @@
         <v>6</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="65">
+      <c r="J26" s="59">
         <v>1.8E-3</v>
       </c>
-      <c r="K26" s="65">
+      <c r="K26" s="59">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="L26" s="65">
+      <c r="L26" s="59">
         <v>5.4399999999999997E-2</v>
       </c>
-      <c r="M26" s="65">
+      <c r="M26" s="59">
         <v>0.1237</v>
       </c>
       <c r="N26" s="2"/>
@@ -1917,8 +1989,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="63"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="73"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -1939,16 +2011,16 @@
         <v>6</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="65">
+      <c r="J27" s="59">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="K27" s="65">
+      <c r="K27" s="59">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="L27" s="65">
+      <c r="L27" s="59">
         <v>5.62E-2</v>
       </c>
-      <c r="M27" s="65">
+      <c r="M27" s="59">
         <v>0.12820000000000001</v>
       </c>
       <c r="N27" s="2"/>
@@ -1958,8 +2030,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="64"/>
-      <c r="R27" s="63"/>
+      <c r="Q27" s="74"/>
+      <c r="R27" s="73"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -1980,16 +2052,16 @@
         <v>6</v>
       </c>
       <c r="I28" s="2"/>
-      <c r="J28" s="67">
+      <c r="J28" s="60">
         <v>7.6E-3</v>
       </c>
-      <c r="K28" s="67">
+      <c r="K28" s="60">
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="L28" s="67">
+      <c r="L28" s="60">
         <v>6.1199999999999997E-2</v>
       </c>
-      <c r="M28" s="67">
+      <c r="M28" s="60">
         <v>0.12180000000000001</v>
       </c>
       <c r="N28" s="2"/>
@@ -1999,8 +2071,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="63"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="73"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2021,16 +2093,16 @@
         <v>6</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="67">
+      <c r="J29" s="60">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="K29" s="67">
+      <c r="K29" s="60">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="L29" s="67">
+      <c r="L29" s="60">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="M29" s="67">
+      <c r="M29" s="60">
         <v>0.1138</v>
       </c>
       <c r="N29" s="2"/>
@@ -2040,8 +2112,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="64"/>
-      <c r="R29" s="63"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="73"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2062,16 +2134,16 @@
         <v>6</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="67">
+      <c r="J30" s="60">
         <v>1.8E-3</v>
       </c>
-      <c r="K30" s="67">
+      <c r="K30" s="60">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="L30" s="67">
+      <c r="L30" s="60">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="M30" s="67">
+      <c r="M30" s="60">
         <v>0.1149</v>
       </c>
       <c r="N30" s="2"/>
@@ -2081,8 +2153,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="64"/>
-      <c r="R30" s="63"/>
+      <c r="Q30" s="74"/>
+      <c r="R30" s="73"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2103,16 +2175,16 @@
         <v>6</v>
       </c>
       <c r="I31" s="2"/>
-      <c r="J31" s="67">
+      <c r="J31" s="60">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="K31" s="67">
+      <c r="K31" s="60">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="L31" s="67">
+      <c r="L31" s="60">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="M31" s="67">
+      <c r="M31" s="60">
         <v>0.1221</v>
       </c>
       <c r="N31" s="2"/>
@@ -2122,8 +2194,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="63"/>
+      <c r="Q31" s="74"/>
+      <c r="R31" s="73"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2144,16 +2216,16 @@
         <v>6</v>
       </c>
       <c r="I32" s="2"/>
-      <c r="J32" s="67">
+      <c r="J32" s="60">
         <v>9.3041E-4</v>
       </c>
-      <c r="K32" s="67">
+      <c r="K32" s="60">
         <v>2.3E-3</v>
       </c>
-      <c r="L32" s="67">
+      <c r="L32" s="60">
         <v>5.7700000000000001E-2</v>
       </c>
-      <c r="M32" s="67">
+      <c r="M32" s="60">
         <v>0.1167</v>
       </c>
       <c r="N32" s="2"/>
@@ -2163,8 +2235,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="63"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="73"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2185,16 +2257,16 @@
         <v>6</v>
       </c>
       <c r="I33" s="2"/>
-      <c r="J33" s="68">
+      <c r="J33" s="61">
         <v>2.3900000000000001E-2</v>
       </c>
-      <c r="K33" s="68">
+      <c r="K33" s="61">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="L33" s="68">
+      <c r="L33" s="61">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="M33" s="68">
+      <c r="M33" s="61">
         <v>0.16020000000000001</v>
       </c>
       <c r="N33" s="2"/>
@@ -2204,8 +2276,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="64"/>
-      <c r="R33" s="63"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="73"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2226,16 +2298,16 @@
         <v>6</v>
       </c>
       <c r="I34" s="2"/>
-      <c r="J34" s="68">
+      <c r="J34" s="61">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="K34" s="68">
+      <c r="K34" s="61">
         <v>1.78E-2</v>
       </c>
-      <c r="L34" s="68">
+      <c r="L34" s="61">
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="M34" s="68">
+      <c r="M34" s="61">
         <v>0.16550000000000001</v>
       </c>
       <c r="N34" s="2"/>
@@ -2245,8 +2317,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="64"/>
-      <c r="R34" s="63"/>
+      <c r="Q34" s="74"/>
+      <c r="R34" s="73"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2267,16 +2339,16 @@
         <v>6</v>
       </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="68">
+      <c r="J35" s="61">
         <v>3.3E-3</v>
       </c>
-      <c r="K35" s="68">
+      <c r="K35" s="61">
         <v>8.2000000000000007E-3</v>
       </c>
-      <c r="L35" s="68">
+      <c r="L35" s="61">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M35" s="68">
+      <c r="M35" s="61">
         <v>0.1643</v>
       </c>
       <c r="N35" s="2"/>
@@ -2286,8 +2358,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="64"/>
-      <c r="R35" s="63"/>
+      <c r="Q35" s="74"/>
+      <c r="R35" s="73"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2308,16 +2380,16 @@
         <v>6</v>
       </c>
       <c r="I36" s="2"/>
-      <c r="J36" s="68">
+      <c r="J36" s="61">
         <v>2E-3</v>
       </c>
-      <c r="K36" s="68">
+      <c r="K36" s="61">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L36" s="68">
+      <c r="L36" s="61">
         <v>5.9200000000000003E-2</v>
       </c>
-      <c r="M36" s="68">
+      <c r="M36" s="61">
         <v>0.1593</v>
       </c>
       <c r="N36" s="2"/>
@@ -2327,8 +2399,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="64"/>
-      <c r="R36" s="63"/>
+      <c r="Q36" s="74"/>
+      <c r="R36" s="73"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2349,16 +2421,16 @@
         <v>6</v>
       </c>
       <c r="I37" s="2"/>
-      <c r="J37" s="68">
+      <c r="J37" s="61">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="K37" s="68">
+      <c r="K37" s="61">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L37" s="68">
+      <c r="L37" s="61">
         <v>5.8900000000000001E-2</v>
       </c>
-      <c r="M37" s="68">
+      <c r="M37" s="61">
         <v>0.15870000000000001</v>
       </c>
       <c r="N37" s="2"/>
@@ -2368,21 +2440,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="64"/>
-      <c r="R37" s="63"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="73"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+      <c r="J39" s="71"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -2446,16 +2518,16 @@
         <v>6</v>
       </c>
       <c r="I41" s="2"/>
-      <c r="J41" s="65">
+      <c r="J41" s="59">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="K41" s="65">
+      <c r="K41" s="59">
         <v>1.41E-2</v>
       </c>
-      <c r="L41" s="65">
+      <c r="L41" s="59">
         <v>5.7299999999999997E-2</v>
       </c>
-      <c r="M41" s="65">
+      <c r="M41" s="59">
         <v>0.13070000000000001</v>
       </c>
       <c r="N41" s="2"/>
@@ -2485,16 +2557,16 @@
         <v>6</v>
       </c>
       <c r="I42" s="2"/>
-      <c r="J42" s="65">
+      <c r="J42" s="59">
         <v>1.4E-3</v>
       </c>
-      <c r="K42" s="65">
+      <c r="K42" s="59">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="L42" s="65">
+      <c r="L42" s="59">
         <v>5.8099999999999999E-2</v>
       </c>
-      <c r="M42" s="65">
+      <c r="M42" s="59">
         <v>0.1323</v>
       </c>
       <c r="N42" s="2"/>
@@ -2524,16 +2596,16 @@
         <v>6</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="65">
+      <c r="J43" s="59">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="K43" s="65">
+      <c r="K43" s="59">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="L43" s="65">
+      <c r="L43" s="59">
         <v>5.5300000000000002E-2</v>
       </c>
-      <c r="M43" s="65">
+      <c r="M43" s="59">
         <v>0.12529999999999999</v>
       </c>
       <c r="N43" s="2"/>
@@ -2563,16 +2635,16 @@
         <v>6</v>
       </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="65">
+      <c r="J44" s="59">
         <v>5.2610999999999999E-4</v>
       </c>
-      <c r="K44" s="65">
+      <c r="K44" s="59">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="L44" s="65">
+      <c r="L44" s="59">
         <v>5.67E-2</v>
       </c>
-      <c r="M44" s="65">
+      <c r="M44" s="59">
         <v>0.129</v>
       </c>
       <c r="N44" s="2"/>
@@ -2602,16 +2674,16 @@
         <v>6</v>
       </c>
       <c r="I45" s="2"/>
-      <c r="J45" s="66">
+      <c r="J45" s="62">
         <v>1.7221000000000001E-4</v>
       </c>
-      <c r="K45" s="66">
+      <c r="K45" s="62">
         <v>4.3927000000000001E-4</v>
       </c>
-      <c r="L45" s="66">
+      <c r="L45" s="62">
         <v>5.7500000000000002E-2</v>
       </c>
-      <c r="M45" s="66">
+      <c r="M45" s="62">
         <v>0.12970000000000001</v>
       </c>
       <c r="N45" s="2"/>
@@ -2641,16 +2713,16 @@
         <v>6</v>
       </c>
       <c r="I46" s="57"/>
-      <c r="J46" s="67">
+      <c r="J46" s="60">
         <v>1.23E-2</v>
       </c>
-      <c r="K46" s="67">
+      <c r="K46" s="60">
         <v>3.1300000000000001E-2</v>
       </c>
-      <c r="L46" s="67">
+      <c r="L46" s="60">
         <v>7.0499999999999993E-2</v>
       </c>
-      <c r="M46" s="67">
+      <c r="M46" s="60">
         <v>0.1484</v>
       </c>
       <c r="N46" s="57"/>
@@ -2680,16 +2752,16 @@
         <v>6</v>
       </c>
       <c r="I47" s="57"/>
-      <c r="J47" s="67">
+      <c r="J47" s="60">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="K47" s="67">
+      <c r="K47" s="60">
         <v>4.3E-3</v>
       </c>
-      <c r="L47" s="67">
+      <c r="L47" s="60">
         <v>6.1899999999999997E-2</v>
       </c>
-      <c r="M47" s="67">
+      <c r="M47" s="60">
         <v>0.1241</v>
       </c>
       <c r="N47" s="57"/>
@@ -2719,16 +2791,16 @@
         <v>6</v>
       </c>
       <c r="I48" s="57"/>
-      <c r="J48" s="67">
+      <c r="J48" s="60">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="K48" s="67">
+      <c r="K48" s="60">
         <v>3.0999999999999999E-3</v>
       </c>
-      <c r="L48" s="67">
+      <c r="L48" s="60">
         <v>6.2799999999999995E-2</v>
       </c>
-      <c r="M48" s="67">
+      <c r="M48" s="60">
         <v>0.1278</v>
       </c>
       <c r="N48" s="57"/>
@@ -2758,16 +2830,16 @@
         <v>6</v>
       </c>
       <c r="I49" s="57"/>
-      <c r="J49" s="67">
+      <c r="J49" s="60">
         <v>8.6755000000000003E-4</v>
       </c>
-      <c r="K49" s="67">
+      <c r="K49" s="60">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="L49" s="67">
+      <c r="L49" s="60">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="M49" s="67">
+      <c r="M49" s="60">
         <v>0.13569999999999999</v>
       </c>
       <c r="N49" s="57"/>
@@ -2797,16 +2869,16 @@
         <v>6</v>
       </c>
       <c r="I50" s="57"/>
-      <c r="J50" s="67">
+      <c r="J50" s="60">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="K50" s="67">
+      <c r="K50" s="60">
         <v>2.8E-3</v>
       </c>
-      <c r="L50" s="67">
+      <c r="L50" s="60">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="M50" s="67">
+      <c r="M50" s="60">
         <v>0.1268</v>
       </c>
       <c r="N50" s="57"/>
@@ -2840,12 +2912,6 @@
       <c r="K54" s="58"/>
       <c r="L54" s="58"/>
       <c r="M54" s="58"/>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J55" s="58"/>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2856,4 +2922,233 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700D6289-7F49-44DE-80C1-CB1E300057D2}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="B5:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="4.28515625" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="78"/>
+      <c r="L5" s="75" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="77">
+        <v>30</v>
+      </c>
+      <c r="D6" s="76">
+        <v>1E-4</v>
+      </c>
+      <c r="E6" s="76">
+        <v>800</v>
+      </c>
+      <c r="F6" s="76">
+        <v>8</v>
+      </c>
+      <c r="G6" s="76">
+        <f>20%*E6</f>
+        <v>160</v>
+      </c>
+      <c r="H6" s="76">
+        <f>80%*800</f>
+        <v>640</v>
+      </c>
+      <c r="I6" s="76">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="79"/>
+      <c r="L6" s="81">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="M6" s="81">
+        <v>0.1246</v>
+      </c>
+      <c r="N6" s="81">
+        <v>6.7400000000000002E-2</v>
+      </c>
+      <c r="O6" s="81">
+        <v>0.14319999999999999</v>
+      </c>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="76">
+        <v>41.19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="76"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="76"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="76"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="76"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="79"/>
+      <c r="Q11" s="76"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K5:K12"/>
+    <mergeCell ref="P5:P12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add - Creación de directorio para guardar modelos
primer modelo guardado .h5
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25135F7-4796-4D64-BC2A-652C6C0B1207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966E4A2E-3E3C-4F1F-A6E3-E12A1D3DC3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="62">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t># inputs</t>
+  </si>
+  <si>
+    <t>unet_model_decay_cosine_1</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,26 +673,29 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2932,217 +2938,219 @@
   <dimension ref="B5:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
     <col min="11" max="11" width="4.28515625" customWidth="1"/>
     <col min="16" max="16" width="4.28515625" customWidth="1"/>
     <col min="17" max="17" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="78"/>
-      <c r="L5" s="75" t="s">
+      <c r="K5" s="77"/>
+      <c r="L5" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="N5" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="75" t="s">
+      <c r="P5" s="77"/>
+      <c r="Q5" s="82" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="77">
+      <c r="B6" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="76">
         <v>30</v>
       </c>
-      <c r="D6" s="76">
-        <v>1E-4</v>
-      </c>
-      <c r="E6" s="76">
+      <c r="D6" s="75">
+        <v>1E-4</v>
+      </c>
+      <c r="E6" s="75">
         <v>800</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="75">
         <v>8</v>
       </c>
-      <c r="G6" s="76">
+      <c r="G6" s="75">
         <f>20%*E6</f>
         <v>160</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="75">
         <f>80%*800</f>
         <v>640</v>
       </c>
-      <c r="I6" s="76">
+      <c r="I6" s="75">
         <v>0.1</v>
       </c>
-      <c r="J6" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="81">
+      <c r="J6" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="78"/>
+      <c r="L6" s="80">
         <v>4.8399999999999999E-2</v>
       </c>
-      <c r="M6" s="81">
+      <c r="M6" s="80">
         <v>0.1246</v>
       </c>
-      <c r="N6" s="81">
+      <c r="N6" s="80">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="O6" s="81">
+      <c r="O6" s="80">
         <v>0.14319999999999999</v>
       </c>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="76">
+      <c r="P6" s="78"/>
+      <c r="Q6" s="75">
         <v>41.19</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="76"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="75"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="79"/>
-      <c r="Q9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="75"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="75"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="79"/>
-      <c r="Q11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="75"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="80"/>
-      <c r="Q12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="79"/>
+      <c r="Q12" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add - Actualización de ambiente tensorflow (myredv2))
- nuevo ambiente:  "myredv2"
- implementación de función Cosine Decay
- análisis de métricas

pd: Falta normalizar datos y si es necesario incrementar los inputs para el entrenamiento.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966E4A2E-3E3C-4F1F-A6E3-E12A1D3DC3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A8F7E8-1E49-46FA-B25D-4DE85DCA6F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="59">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -210,19 +210,10 @@
     <t>batch_size</t>
   </si>
   <si>
-    <t>warm_steps(20%)</t>
-  </si>
-  <si>
-    <t>decay_steps (80%)</t>
-  </si>
-  <si>
     <t>tiempo de entrenamiento (min)</t>
   </si>
   <si>
     <t># inputs</t>
-  </si>
-  <si>
-    <t>unet_model_decay_cosine_1</t>
   </si>
 </sst>
 </file>
@@ -655,6 +646,21 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -673,12 +679,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,15 +687,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1042,48 +1033,48 @@
   </sheetPr>
   <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:J55"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
     <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="14" max="14" width="4.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-    </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+    </row>
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-    </row>
-    <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+    </row>
+    <row r="4" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1169,7 +1160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
@@ -1241,7 +1232,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
@@ -1282,7 +1273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1314,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>24</v>
       </c>
@@ -1364,7 +1355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1396,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
@@ -1446,7 +1437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
@@ -1487,7 +1478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>27</v>
       </c>
@@ -1528,7 +1519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>28</v>
       </c>
@@ -1569,7 +1560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>29</v>
       </c>
@@ -1610,7 +1601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>30</v>
       </c>
@@ -1651,7 +1642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
@@ -1692,7 +1683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>32</v>
       </c>
@@ -1733,7 +1724,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>33</v>
       </c>
@@ -1774,7 +1765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>34</v>
       </c>
@@ -1815,7 +1806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -1832,7 +1823,7 @@
       <c r="O22" s="47"/>
       <c r="P22" s="33"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="s">
         <v>35</v>
       </c>
@@ -1870,12 +1861,12 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="72" t="s">
+      <c r="Q23" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="73"/>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="78"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
         <v>36</v>
       </c>
@@ -1913,10 +1904,10 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="74"/>
-      <c r="R24" s="73"/>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="79"/>
+      <c r="R24" s="78"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
         <v>37</v>
       </c>
@@ -1954,10 +1945,10 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="73"/>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q25" s="79"/>
+      <c r="R25" s="78"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>38</v>
       </c>
@@ -1995,10 +1986,10 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="74"/>
-      <c r="R26" s="73"/>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q26" s="79"/>
+      <c r="R26" s="78"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="29" t="s">
         <v>39</v>
       </c>
@@ -2036,10 +2027,10 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="74"/>
-      <c r="R27" s="73"/>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q27" s="79"/>
+      <c r="R27" s="78"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="18" t="s">
         <v>35</v>
       </c>
@@ -2077,10 +2068,10 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="74"/>
-      <c r="R28" s="73"/>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q28" s="79"/>
+      <c r="R28" s="78"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="18" t="s">
         <v>36</v>
       </c>
@@ -2118,10 +2109,10 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="73"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q29" s="79"/>
+      <c r="R29" s="78"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
         <v>37</v>
       </c>
@@ -2159,10 +2150,10 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="73"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q30" s="79"/>
+      <c r="R30" s="78"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
         <v>38</v>
       </c>
@@ -2200,10 +2191,10 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="73"/>
-    </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q31" s="79"/>
+      <c r="R31" s="78"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="29" t="s">
         <v>39</v>
       </c>
@@ -2241,10 +2232,10 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="73"/>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q32" s="79"/>
+      <c r="R32" s="78"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
         <v>35</v>
       </c>
@@ -2282,10 +2273,10 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="73"/>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q33" s="79"/>
+      <c r="R33" s="78"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
         <v>36</v>
       </c>
@@ -2323,10 +2314,10 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="73"/>
-    </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q34" s="79"/>
+      <c r="R34" s="78"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
         <v>37</v>
       </c>
@@ -2364,10 +2355,10 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="73"/>
-    </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q35" s="79"/>
+      <c r="R35" s="78"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="18" t="s">
         <v>38</v>
       </c>
@@ -2405,10 +2396,10 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="74"/>
-      <c r="R36" s="73"/>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q36" s="79"/>
+      <c r="R36" s="78"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B37" s="29" t="s">
         <v>39</v>
       </c>
@@ -2446,23 +2437,23 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="73"/>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="71" t="s">
+      <c r="Q37" s="79"/>
+      <c r="R37" s="78"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B39" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
-    </row>
-    <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+    </row>
+    <row r="40" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B40" s="49" t="s">
         <v>5</v>
       </c>
@@ -2505,7 +2496,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B41" s="29" t="s">
         <v>43</v>
       </c>
@@ -2544,7 +2535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B42" s="29" t="s">
         <v>44</v>
       </c>
@@ -2583,7 +2574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B43" s="29" t="s">
         <v>45</v>
       </c>
@@ -2622,7 +2613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B44" s="29" t="s">
         <v>46</v>
       </c>
@@ -2661,7 +2652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
         <v>47</v>
       </c>
@@ -2700,7 +2691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B46" s="18" t="s">
         <v>48</v>
       </c>
@@ -2739,7 +2730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B47" s="18" t="s">
         <v>49</v>
       </c>
@@ -2778,7 +2769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B48" s="18" t="s">
         <v>50</v>
       </c>
@@ -2817,7 +2808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
         <v>51</v>
       </c>
@@ -2856,7 +2847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" s="18" t="s">
         <v>52</v>
       </c>
@@ -2895,25 +2886,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J51" s="58"/>
       <c r="K51" s="58"/>
       <c r="L51" s="58"/>
       <c r="M51" s="58"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J52" s="58"/>
       <c r="K52" s="58"/>
       <c r="L52" s="58"/>
       <c r="M52" s="58"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J53" s="58"/>
       <c r="K53" s="58"/>
       <c r="L53" s="58"/>
       <c r="M53" s="58"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J54" s="58"/>
       <c r="K54" s="58"/>
       <c r="L54" s="58"/>
@@ -2935,227 +2926,214 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B5:Q12"/>
+  <dimension ref="B5:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="82" t="s">
+    <row r="5" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="82" t="s">
+      <c r="C5" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="80"/>
+      <c r="K5" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="80"/>
+      <c r="P5" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="82" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="77"/>
-      <c r="L5" s="82" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="82" t="s">
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="70">
+        <v>30</v>
+      </c>
+      <c r="D6" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="E6" s="69">
+        <v>500</v>
+      </c>
+      <c r="F6" s="69">
         <v>8</v>
       </c>
-      <c r="N5" s="82" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="82" t="s">
-        <v>10</v>
-      </c>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="82" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="76">
-        <v>30</v>
-      </c>
-      <c r="D6" s="75">
-        <v>1E-4</v>
-      </c>
-      <c r="E6" s="75">
-        <v>800</v>
-      </c>
-      <c r="F6" s="75">
-        <v>8</v>
-      </c>
-      <c r="G6" s="75">
-        <f>20%*E6</f>
-        <v>160</v>
-      </c>
-      <c r="H6" s="75">
+      <c r="G6" s="69">
         <f>80%*800</f>
         <v>640</v>
       </c>
-      <c r="I6" s="75">
+      <c r="H6" s="69">
         <v>0.1</v>
       </c>
-      <c r="J6" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="78"/>
-      <c r="L6" s="80">
-        <v>4.8399999999999999E-2</v>
-      </c>
-      <c r="M6" s="80">
-        <v>0.1246</v>
-      </c>
-      <c r="N6" s="80">
-        <v>6.7400000000000002E-2</v>
-      </c>
-      <c r="O6" s="80">
-        <v>0.14319999999999999</v>
-      </c>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="75">
-        <v>41.19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="75"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="75"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="75"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="80"/>
-      <c r="O10" s="80"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="75"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="75"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="80"/>
-      <c r="P12" s="79"/>
-      <c r="Q12" s="75"/>
+      <c r="I6" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="81"/>
+      <c r="K6" s="71">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="L6" s="71">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="M6" s="71">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="N6" s="71">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="O6" s="81"/>
+      <c r="P6" s="69">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="69"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="69"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="69"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="69"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="69"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K5:K12"/>
-    <mergeCell ref="P5:P12"/>
+    <mergeCell ref="J5:J12"/>
+    <mergeCell ref="O5:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing - modelos con z-core
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5B8EA9-93CC-4708-B315-AFE90C6992C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B40F03-73B0-4D99-8E47-DDA2B1EA4090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="5295" yWindow="6360" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="60">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -198,9 +198,6 @@
     <t>modelo 32</t>
   </si>
   <si>
-    <t>alpha</t>
-  </si>
-  <si>
     <t>model/hip</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t># inputs</t>
+  </si>
+  <si>
+    <t>modelo 2 - norm z-core</t>
+  </si>
+  <si>
+    <t>modelo 3 - norm z-core</t>
   </si>
 </sst>
 </file>
@@ -1037,31 +1040,31 @@
       <selection activeCell="A28" sqref="A28:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="3.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
-    <col min="14" max="14" width="4.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="4.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="74" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="74"/>
       <c r="D2" s="74"/>
     </row>
-    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="75" t="s">
         <v>40</v>
       </c>
@@ -1074,7 +1077,7 @@
       <c r="I3" s="75"/>
       <c r="J3" s="75"/>
     </row>
-    <row r="4" spans="2:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>22</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>23</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>24</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>28</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>29</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>30</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>32</v>
       </c>
@@ -1724,7 +1727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>33</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>34</v>
       </c>
@@ -1806,7 +1809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -1823,7 +1826,7 @@
       <c r="O22" s="47"/>
       <c r="P22" s="33"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>35</v>
       </c>
@@ -1866,7 +1869,7 @@
       </c>
       <c r="R23" s="78"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>36</v>
       </c>
@@ -1907,7 +1910,7 @@
       <c r="Q24" s="79"/>
       <c r="R24" s="78"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>37</v>
       </c>
@@ -1948,7 +1951,7 @@
       <c r="Q25" s="79"/>
       <c r="R25" s="78"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
         <v>38</v>
       </c>
@@ -1989,7 +1992,7 @@
       <c r="Q26" s="79"/>
       <c r="R26" s="78"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
         <v>39</v>
       </c>
@@ -2030,7 +2033,7 @@
       <c r="Q27" s="79"/>
       <c r="R27" s="78"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
         <v>35</v>
       </c>
@@ -2071,7 +2074,7 @@
       <c r="Q28" s="79"/>
       <c r="R28" s="78"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>36</v>
       </c>
@@ -2112,7 +2115,7 @@
       <c r="Q29" s="79"/>
       <c r="R29" s="78"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
         <v>37</v>
       </c>
@@ -2153,7 +2156,7 @@
       <c r="Q30" s="79"/>
       <c r="R30" s="78"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>38</v>
       </c>
@@ -2194,7 +2197,7 @@
       <c r="Q31" s="79"/>
       <c r="R31" s="78"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
         <v>39</v>
       </c>
@@ -2235,7 +2238,7 @@
       <c r="Q32" s="79"/>
       <c r="R32" s="78"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
         <v>35</v>
       </c>
@@ -2276,7 +2279,7 @@
       <c r="Q33" s="79"/>
       <c r="R33" s="78"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>36</v>
       </c>
@@ -2317,7 +2320,7 @@
       <c r="Q34" s="79"/>
       <c r="R34" s="78"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>37</v>
       </c>
@@ -2358,7 +2361,7 @@
       <c r="Q35" s="79"/>
       <c r="R35" s="78"/>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
         <v>38</v>
       </c>
@@ -2399,7 +2402,7 @@
       <c r="Q36" s="79"/>
       <c r="R36" s="78"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
         <v>39</v>
       </c>
@@ -2440,7 +2443,7 @@
       <c r="Q37" s="79"/>
       <c r="R37" s="78"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="76" t="s">
         <v>42</v>
       </c>
@@ -2453,7 +2456,7 @@
       <c r="I39" s="76"/>
       <c r="J39" s="76"/>
     </row>
-    <row r="40" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
         <v>5</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="29" t="s">
         <v>43</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="29" t="s">
         <v>44</v>
       </c>
@@ -2574,7 +2577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="29" t="s">
         <v>45</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="29" t="s">
         <v>46</v>
       </c>
@@ -2652,7 +2655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>47</v>
       </c>
@@ -2691,7 +2694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>48</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>49</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="18" t="s">
         <v>50</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>51</v>
       </c>
@@ -2847,7 +2850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>52</v>
       </c>
@@ -2886,25 +2889,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J51" s="58"/>
       <c r="K51" s="58"/>
       <c r="L51" s="58"/>
       <c r="M51" s="58"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J52" s="58"/>
       <c r="K52" s="58"/>
       <c r="L52" s="58"/>
       <c r="M52" s="58"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J53" s="58"/>
       <c r="K53" s="58"/>
       <c r="L53" s="58"/>
       <c r="M53" s="58"/>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J54" s="58"/>
       <c r="K54" s="58"/>
       <c r="L54" s="58"/>
@@ -2926,65 +2929,62 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B5:P12"/>
+  <dimension ref="B5:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" customWidth="1"/>
-    <col min="15" max="15" width="4.33203125" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="73" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="73" t="s">
         <v>55</v>
-      </c>
-      <c r="F5" s="73" t="s">
-        <v>56</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="73" t="s">
+        <v>7</v>
+      </c>
       <c r="K5" s="73" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L5" s="73" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M5" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="80"/>
-      <c r="P5" s="73" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N5" s="80"/>
+      <c r="O5" s="73" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="72" t="s">
         <v>1</v>
       </c>
@@ -3001,68 +3001,103 @@
         <v>8</v>
       </c>
       <c r="G6" s="69">
-        <f>80%*800</f>
-        <v>640</v>
-      </c>
-      <c r="H6" s="69">
-        <v>0.1</v>
-      </c>
-      <c r="I6" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="81"/>
+        <f>80%*E6</f>
+        <v>400</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="81"/>
+      <c r="J6" s="71">
+        <v>7.1400000000000005E-2</v>
+      </c>
       <c r="K6" s="71">
-        <v>7.1400000000000005E-2</v>
+        <v>0.18490000000000001</v>
       </c>
       <c r="L6" s="71">
-        <v>0.18490000000000001</v>
+        <v>7.4399999999999994E-2</v>
       </c>
       <c r="M6" s="71">
-        <v>7.4399999999999994E-2</v>
-      </c>
-      <c r="N6" s="71">
         <v>0.16400000000000001</v>
       </c>
-      <c r="O6" s="81"/>
-      <c r="P6" s="69">
+      <c r="N6" s="81"/>
+      <c r="O6" s="69">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="69"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="81"/>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="70">
+        <v>30</v>
+      </c>
+      <c r="D7" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="E7" s="69">
+        <v>500</v>
+      </c>
+      <c r="F7" s="69">
+        <v>8</v>
+      </c>
+      <c r="G7" s="69">
+        <f>80%*E7</f>
+        <v>400</v>
+      </c>
+      <c r="H7" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="81"/>
+      <c r="J7" s="71">
+        <v>4.5789</v>
+      </c>
+      <c r="K7" s="71">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="L7" s="71">
+        <v>4.1780999999999997</v>
+      </c>
+      <c r="M7" s="71">
+        <v>0.2122</v>
+      </c>
+      <c r="N7" s="81"/>
+      <c r="O7" s="69">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="70">
+        <v>30</v>
+      </c>
+      <c r="D8" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="E8" s="69">
+        <v>410</v>
+      </c>
+      <c r="F8" s="69">
+        <v>8</v>
+      </c>
+      <c r="G8" s="69">
+        <f>80%*E8</f>
+        <v>328</v>
+      </c>
+      <c r="H8" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="81"/>
+      <c r="J8" s="71"/>
       <c r="K8" s="71"/>
       <c r="L8" s="71"/>
       <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="69"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N8" s="81"/>
+      <c r="O8" s="69"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="70"/>
       <c r="C9" s="70"/>
       <c r="D9" s="69"/>
@@ -3070,16 +3105,15 @@
       <c r="F9" s="69"/>
       <c r="G9" s="69"/>
       <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="71"/>
       <c r="K9" s="71"/>
       <c r="L9" s="71"/>
       <c r="M9" s="71"/>
-      <c r="N9" s="71"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="69"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N9" s="81"/>
+      <c r="O9" s="69"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
       <c r="D10" s="69"/>
@@ -3087,16 +3121,15 @@
       <c r="F10" s="69"/>
       <c r="G10" s="69"/>
       <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="71"/>
       <c r="K10" s="71"/>
       <c r="L10" s="71"/>
       <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="69"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N10" s="81"/>
+      <c r="O10" s="69"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
       <c r="D11" s="69"/>
@@ -3104,16 +3137,15 @@
       <c r="F11" s="69"/>
       <c r="G11" s="69"/>
       <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="71"/>
       <c r="K11" s="71"/>
       <c r="L11" s="71"/>
       <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="69"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N11" s="81"/>
+      <c r="O11" s="69"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
       <c r="D12" s="69"/>
@@ -3121,19 +3153,18 @@
       <c r="F12" s="69"/>
       <c r="G12" s="69"/>
       <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="71"/>
       <c r="K12" s="71"/>
       <c r="L12" s="71"/>
       <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="69"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J5:J12"/>
-    <mergeCell ref="O5:O12"/>
+    <mergeCell ref="I5:I12"/>
+    <mergeCell ref="N5:N12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing - hiperparametros y norm z-core
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B40F03-73B0-4D99-8E47-DDA2B1EA4090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7155CF40-6497-43E4-8687-3B37830BAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="6360" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="4965" yWindow="6855" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="64">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>modelo 3 - norm z-core</t>
+  </si>
+  <si>
+    <t>modelo 4 - norm z-core</t>
+  </si>
+  <si>
+    <t>70/30</t>
+  </si>
+  <si>
+    <t>80/20</t>
+  </si>
+  <si>
+    <t>train y val (%)</t>
   </si>
 </sst>
 </file>
@@ -2929,22 +2941,23 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B5:O12"/>
+  <dimension ref="B5:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" customWidth="1"/>
-    <col min="15" max="15" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="73" t="s">
         <v>53</v>
       </c>
@@ -2952,219 +2965,262 @@
         <v>57</v>
       </c>
       <c r="D5" s="73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="F5" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="G5" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="H5" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="I5" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="80"/>
+      <c r="K5" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="L5" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="73" t="s">
+      <c r="M5" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="73" t="s">
+      <c r="N5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="80"/>
-      <c r="O5" s="73" t="s">
+      <c r="O5" s="80"/>
+      <c r="P5" s="73" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="72" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="70">
         <v>30</v>
       </c>
-      <c r="D6" s="69">
-        <v>1E-4</v>
+      <c r="D6" s="70" t="s">
+        <v>61</v>
       </c>
       <c r="E6" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="F6" s="69">
         <v>500</v>
       </c>
-      <c r="F6" s="69">
+      <c r="G6" s="69">
         <v>8</v>
       </c>
-      <c r="G6" s="69">
-        <f>80%*E6</f>
+      <c r="H6" s="69">
+        <f>80%*F6</f>
         <v>400</v>
       </c>
-      <c r="H6" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="71">
+      <c r="I6" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="81"/>
+      <c r="K6" s="71">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="K6" s="71">
+      <c r="L6" s="71">
         <v>0.18490000000000001</v>
       </c>
-      <c r="L6" s="71">
+      <c r="M6" s="71">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="M6" s="71">
+      <c r="N6" s="71">
         <v>0.16400000000000001</v>
       </c>
-      <c r="N6" s="81"/>
-      <c r="O6" s="69">
+      <c r="O6" s="81"/>
+      <c r="P6" s="69">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="70" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="70">
         <v>30</v>
       </c>
-      <c r="D7" s="69">
-        <v>1E-4</v>
+      <c r="D7" s="70" t="s">
+        <v>61</v>
       </c>
       <c r="E7" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="69">
         <v>500</v>
       </c>
-      <c r="F7" s="69">
+      <c r="G7" s="69">
         <v>8</v>
       </c>
-      <c r="G7" s="69">
-        <f>80%*E7</f>
+      <c r="H7" s="69">
+        <f>80%*F7</f>
         <v>400</v>
       </c>
-      <c r="H7" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="71">
+      <c r="I7" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="81"/>
+      <c r="K7" s="71">
         <v>4.5789</v>
       </c>
-      <c r="K7" s="71">
+      <c r="L7" s="71">
         <v>0.25600000000000001</v>
       </c>
-      <c r="L7" s="71">
+      <c r="M7" s="71">
         <v>4.1780999999999997</v>
       </c>
-      <c r="M7" s="71">
+      <c r="N7" s="71">
         <v>0.2122</v>
       </c>
-      <c r="N7" s="81"/>
-      <c r="O7" s="69">
+      <c r="O7" s="81"/>
+      <c r="P7" s="69">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="70" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="70">
         <v>30</v>
       </c>
-      <c r="D8" s="69">
-        <v>1E-4</v>
+      <c r="D8" s="70" t="s">
+        <v>61</v>
       </c>
       <c r="E8" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="69">
         <v>410</v>
       </c>
-      <c r="F8" s="69">
+      <c r="G8" s="69">
         <v>8</v>
       </c>
-      <c r="G8" s="69">
-        <f>80%*E8</f>
+      <c r="H8" s="69">
+        <f>80%*F8</f>
         <v>328</v>
       </c>
-      <c r="H8" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="81"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="69"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="71"/>
+      <c r="I8" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="81"/>
+      <c r="K8" s="71">
+        <v>6.4744999999999999</v>
+      </c>
+      <c r="L8" s="71">
+        <v>0.36609999999999998</v>
+      </c>
+      <c r="M8" s="71">
+        <v>5.7979000000000003</v>
+      </c>
+      <c r="N8" s="71">
+        <v>0.30930000000000002</v>
+      </c>
+      <c r="O8" s="81"/>
+      <c r="P8" s="69">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="70">
+        <v>30</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="69">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F9" s="69">
+        <v>500</v>
+      </c>
+      <c r="G9" s="69">
+        <v>8</v>
+      </c>
+      <c r="H9" s="69">
+        <f>80%*F9</f>
+        <v>400</v>
+      </c>
+      <c r="I9" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="81"/>
       <c r="K9" s="71"/>
       <c r="L9" s="71"/>
       <c r="M9" s="71"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="69"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="71"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="69"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
-      <c r="D10" s="69"/>
+      <c r="D10" s="70"/>
       <c r="E10" s="69"/>
       <c r="F10" s="69"/>
       <c r="G10" s="69"/>
       <c r="H10" s="69"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="71"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="81"/>
       <c r="K10" s="71"/>
       <c r="L10" s="71"/>
       <c r="M10" s="71"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="69"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="71"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="69"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
-      <c r="D11" s="69"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="69"/>
       <c r="F11" s="69"/>
       <c r="G11" s="69"/>
       <c r="H11" s="69"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="71"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="81"/>
       <c r="K11" s="71"/>
       <c r="L11" s="71"/>
       <c r="M11" s="71"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="69"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N11" s="71"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="69"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
-      <c r="D12" s="69"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="69"/>
       <c r="F12" s="69"/>
       <c r="G12" s="69"/>
       <c r="H12" s="69"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="71"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="82"/>
       <c r="K12" s="71"/>
       <c r="L12" s="71"/>
       <c r="M12" s="71"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="69"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I5:I12"/>
-    <mergeCell ref="N5:N12"/>
+    <mergeCell ref="J5:J12"/>
+    <mergeCell ref="O5:O12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add - inputs aumento 30->50 e implementación de normalización min-max
Se obtendrán métricas de esta normalización "min-max" para compararlas con la normalización "z-core" implementada anteriormente.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7155CF40-6497-43E4-8687-3B37830BAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E14E43D-07AF-45C9-B6DE-C18C6EFA47A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="6855" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="3495" yWindow="4800" windowWidth="21600" windowHeight="9075" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>train y val (%)</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_z-core_1.keras</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +392,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -463,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -661,18 +670,6 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -695,13 +692,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,24 +1082,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1876,10 +1888,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="77" t="s">
+      <c r="Q23" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="78"/>
+      <c r="R23" s="74"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1919,8 +1931,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="78"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="74"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -1960,8 +1972,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="78"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="74"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2001,8 +2013,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="78"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="74"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2042,8 +2054,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="78"/>
+      <c r="Q27" s="75"/>
+      <c r="R27" s="74"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2083,8 +2095,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="79"/>
-      <c r="R28" s="78"/>
+      <c r="Q28" s="75"/>
+      <c r="R28" s="74"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2124,8 +2136,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="79"/>
-      <c r="R29" s="78"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="74"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2165,8 +2177,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="79"/>
-      <c r="R30" s="78"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="74"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2206,8 +2218,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="79"/>
-      <c r="R31" s="78"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="74"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2247,8 +2259,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="79"/>
-      <c r="R32" s="78"/>
+      <c r="Q32" s="75"/>
+      <c r="R32" s="74"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2288,8 +2300,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="79"/>
-      <c r="R33" s="78"/>
+      <c r="Q33" s="75"/>
+      <c r="R33" s="74"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2329,8 +2341,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="79"/>
-      <c r="R34" s="78"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="74"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2370,8 +2382,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="78"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="74"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2411,8 +2423,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="79"/>
-      <c r="R36" s="78"/>
+      <c r="Q36" s="75"/>
+      <c r="R36" s="74"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2452,21 +2464,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="78"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="74"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="76" t="s">
+      <c r="B39" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -2944,278 +2956,316 @@
   <dimension ref="B5:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
     <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="73" t="s">
+      <c r="I5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="80"/>
-      <c r="K5" s="73" t="s">
+      <c r="J5" s="76"/>
+      <c r="K5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="73" t="s">
+      <c r="L5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="73" t="s">
+      <c r="M5" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="73" t="s">
+      <c r="N5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="80"/>
-      <c r="P5" s="73" t="s">
+      <c r="O5" s="76"/>
+      <c r="P5" s="69" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="77">
         <v>30</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="69">
-        <v>1E-4</v>
-      </c>
-      <c r="F6" s="69">
+      <c r="E6" s="78">
+        <v>1E-4</v>
+      </c>
+      <c r="F6" s="78">
         <v>500</v>
       </c>
-      <c r="G6" s="69">
+      <c r="G6" s="78">
         <v>8</v>
       </c>
-      <c r="H6" s="69">
+      <c r="H6" s="78">
         <f>80%*F6</f>
         <v>400</v>
       </c>
-      <c r="I6" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="81"/>
-      <c r="K6" s="71">
+      <c r="I6" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="79"/>
+      <c r="K6" s="80">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="L6" s="71">
+      <c r="L6" s="80">
         <v>0.18490000000000001</v>
       </c>
-      <c r="M6" s="71">
+      <c r="M6" s="80">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="N6" s="71">
+      <c r="N6" s="80">
         <v>0.16400000000000001</v>
       </c>
-      <c r="O6" s="81"/>
-      <c r="P6" s="69">
+      <c r="O6" s="79"/>
+      <c r="P6" s="78">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="70">
+      <c r="C7" s="77">
         <v>30</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="69">
-        <v>1E-4</v>
-      </c>
-      <c r="F7" s="69">
+      <c r="E7" s="78">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="78">
         <v>500</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="78">
         <v>8</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="78">
         <f>80%*F7</f>
         <v>400</v>
       </c>
-      <c r="I7" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="71">
+      <c r="I7" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="79"/>
+      <c r="K7" s="80">
         <v>4.5789</v>
       </c>
-      <c r="L7" s="71">
+      <c r="L7" s="80">
         <v>0.25600000000000001</v>
       </c>
-      <c r="M7" s="71">
+      <c r="M7" s="80">
         <v>4.1780999999999997</v>
       </c>
-      <c r="N7" s="71">
+      <c r="N7" s="80">
         <v>0.2122</v>
       </c>
-      <c r="O7" s="81"/>
-      <c r="P7" s="69">
+      <c r="O7" s="79"/>
+      <c r="P7" s="78">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="70">
+      <c r="C8" s="77">
         <v>30</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="69">
-        <v>1E-4</v>
-      </c>
-      <c r="F8" s="69">
+      <c r="E8" s="78">
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="78">
         <v>410</v>
       </c>
-      <c r="G8" s="69">
+      <c r="G8" s="78">
         <v>8</v>
       </c>
-      <c r="H8" s="69">
+      <c r="H8" s="78">
         <f>80%*F8</f>
         <v>328</v>
       </c>
-      <c r="I8" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="81"/>
-      <c r="K8" s="71">
+      <c r="I8" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="79"/>
+      <c r="K8" s="80">
         <v>6.4744999999999999</v>
       </c>
-      <c r="L8" s="71">
+      <c r="L8" s="80">
         <v>0.36609999999999998</v>
       </c>
-      <c r="M8" s="71">
+      <c r="M8" s="80">
         <v>5.7979000000000003</v>
       </c>
-      <c r="N8" s="71">
+      <c r="N8" s="80">
         <v>0.30930000000000002</v>
       </c>
-      <c r="O8" s="81"/>
-      <c r="P8" s="69">
+      <c r="O8" s="79"/>
+      <c r="P8" s="78">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="70">
+      <c r="C9" s="77">
         <v>30</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="69">
+      <c r="E9" s="78">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F9" s="78">
         <v>500</v>
       </c>
-      <c r="G9" s="69">
+      <c r="G9" s="78">
         <v>8</v>
       </c>
-      <c r="H9" s="69">
+      <c r="H9" s="78">
         <f>80%*F9</f>
         <v>400</v>
       </c>
-      <c r="I9" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="81"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
-      <c r="N9" s="71"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="69"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="69"/>
+      <c r="I9" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="79"/>
+      <c r="K9" s="80">
+        <v>8.9992000000000001</v>
+      </c>
+      <c r="L9" s="80">
+        <v>0.50509999999999999</v>
+      </c>
+      <c r="M9" s="80">
+        <v>7.8844000000000003</v>
+      </c>
+      <c r="N9" s="80">
+        <v>0.46489999999999998</v>
+      </c>
+      <c r="O9" s="79"/>
+      <c r="P9" s="78">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="77">
+        <v>50</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="78">
+        <v>1E-4</v>
+      </c>
+      <c r="F10" s="78">
+        <v>400</v>
+      </c>
+      <c r="G10" s="78">
+        <v>8</v>
+      </c>
+      <c r="H10" s="78">
+        <f>80%*F10</f>
+        <v>320</v>
+      </c>
+      <c r="I10" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="79"/>
+      <c r="K10" s="80">
+        <v>4.3776000000000002</v>
+      </c>
+      <c r="L10" s="80">
+        <v>0.25919999999999999</v>
+      </c>
+      <c r="M10" s="80">
+        <v>4.6177000000000001</v>
+      </c>
+      <c r="N10" s="80">
+        <v>0.25719999999999998</v>
+      </c>
+      <c r="O10" s="79"/>
+      <c r="P10" s="78">
+        <v>179</v>
+      </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="69"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="78"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="69"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add - guardado de modelos generados
se define alpha para el dacaimiento de lr usando func.coseno. Mañana se probará los modelos para q hagan predicción,
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E14E43D-07AF-45C9-B6DE-C18C6EFA47A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0B2F43-2AE9-4B43-9DD7-75A408CBEE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="4800" windowWidth="21600" windowHeight="9075" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="4440" yWindow="4440" windowWidth="21600" windowHeight="9075" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="73">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -232,6 +232,50 @@
   </si>
   <si>
     <t>unet_model_decay_coseno_with_normalization_z-core_1.keras</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_minmax_1.keras</t>
+  </si>
+  <si>
+    <t>normalización</t>
+  </si>
+  <si>
+    <t>z-core</t>
+  </si>
+  <si>
+    <t>min-max</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_minmax_2.keras</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>decay_steps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =(#inputs / batch_size) * max_epoch</t>
+    </r>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_minmax_3.keras</t>
   </si>
 </sst>
 </file>
@@ -399,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -455,19 +499,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -670,6 +701,9 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,9 +738,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1082,24 +1113,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1888,10 +1919,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="73" t="s">
+      <c r="Q23" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="74"/>
+      <c r="R23" s="75"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1931,8 +1962,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="74"/>
+      <c r="Q24" s="76"/>
+      <c r="R24" s="75"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -1972,8 +2003,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="75"/>
-      <c r="R25" s="74"/>
+      <c r="Q25" s="76"/>
+      <c r="R25" s="75"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2013,8 +2044,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="75"/>
-      <c r="R26" s="74"/>
+      <c r="Q26" s="76"/>
+      <c r="R26" s="75"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2054,8 +2085,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="75"/>
-      <c r="R27" s="74"/>
+      <c r="Q27" s="76"/>
+      <c r="R27" s="75"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2095,8 +2126,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="75"/>
-      <c r="R28" s="74"/>
+      <c r="Q28" s="76"/>
+      <c r="R28" s="75"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2136,8 +2167,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="75"/>
-      <c r="R29" s="74"/>
+      <c r="Q29" s="76"/>
+      <c r="R29" s="75"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2177,8 +2208,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="75"/>
-      <c r="R30" s="74"/>
+      <c r="Q30" s="76"/>
+      <c r="R30" s="75"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2218,8 +2249,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="75"/>
-      <c r="R31" s="74"/>
+      <c r="Q31" s="76"/>
+      <c r="R31" s="75"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2259,8 +2290,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="74"/>
+      <c r="Q32" s="76"/>
+      <c r="R32" s="75"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2300,8 +2331,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="74"/>
+      <c r="Q33" s="76"/>
+      <c r="R33" s="75"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2341,8 +2372,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="74"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="75"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2382,8 +2413,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="75"/>
-      <c r="R35" s="74"/>
+      <c r="Q35" s="76"/>
+      <c r="R35" s="75"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2423,8 +2454,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="75"/>
-      <c r="R36" s="74"/>
+      <c r="Q36" s="76"/>
+      <c r="R36" s="75"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2464,21 +2495,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="74"/>
+      <c r="Q37" s="76"/>
+      <c r="R37" s="75"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -2953,324 +2984,585 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B5:P12"/>
+  <dimension ref="B3:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="69" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="71"/>
+    </row>
+    <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="G5" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="H5" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="I5" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="K5" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="76"/>
-      <c r="K5" s="69" t="s">
+      <c r="L5" s="77"/>
+      <c r="M5" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="N5" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="69" t="s">
+      <c r="O5" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="69" t="s">
+      <c r="P5" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="76"/>
-      <c r="P5" s="69" t="s">
+      <c r="Q5" s="77"/>
+      <c r="R5" s="70" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="77">
+      <c r="C6" s="78">
         <v>30</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="78">
-        <v>1E-4</v>
-      </c>
-      <c r="F6" s="78">
+      <c r="E6" s="78"/>
+      <c r="F6" s="79">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="79">
         <v>500</v>
       </c>
-      <c r="G6" s="78">
+      <c r="H6" s="79">
         <v>8</v>
       </c>
-      <c r="H6" s="78">
-        <f>80%*F6</f>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79">
+        <f>80%*G6</f>
         <v>400</v>
       </c>
-      <c r="I6" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="79"/>
-      <c r="K6" s="80">
+      <c r="K6" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="80"/>
+      <c r="M6" s="81">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="L6" s="80">
+      <c r="N6" s="81">
         <v>0.18490000000000001</v>
       </c>
-      <c r="M6" s="80">
+      <c r="O6" s="81">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="N6" s="80">
+      <c r="P6" s="81">
         <v>0.16400000000000001</v>
       </c>
-      <c r="O6" s="79"/>
-      <c r="P6" s="78">
+      <c r="Q6" s="80"/>
+      <c r="R6" s="79">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="77">
+      <c r="C7" s="78">
         <v>30</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="78">
-        <v>1E-4</v>
-      </c>
-      <c r="F7" s="78">
+      <c r="E7" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="79">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="79">
         <v>500</v>
       </c>
-      <c r="G7" s="78">
+      <c r="H7" s="79">
         <v>8</v>
       </c>
-      <c r="H7" s="78">
-        <f>80%*F7</f>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79">
+        <f>80%*G7</f>
         <v>400</v>
       </c>
-      <c r="I7" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="79"/>
-      <c r="K7" s="80">
+      <c r="K7" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="80"/>
+      <c r="M7" s="81">
         <v>4.5789</v>
       </c>
-      <c r="L7" s="80">
+      <c r="N7" s="81">
         <v>0.25600000000000001</v>
       </c>
-      <c r="M7" s="80">
+      <c r="O7" s="81">
         <v>4.1780999999999997</v>
       </c>
-      <c r="N7" s="80">
+      <c r="P7" s="81">
         <v>0.2122</v>
       </c>
-      <c r="O7" s="79"/>
-      <c r="P7" s="78">
+      <c r="Q7" s="80"/>
+      <c r="R7" s="79">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="77">
+      <c r="C8" s="78">
         <v>30</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="78">
-        <v>1E-4</v>
-      </c>
-      <c r="F8" s="78">
+      <c r="E8" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="79">
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="79">
         <v>410</v>
       </c>
-      <c r="G8" s="78">
+      <c r="H8" s="79">
         <v>8</v>
       </c>
-      <c r="H8" s="78">
-        <f>80%*F8</f>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79">
+        <f>80%*G8</f>
         <v>328</v>
       </c>
-      <c r="I8" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="79"/>
-      <c r="K8" s="80">
+      <c r="K8" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="80"/>
+      <c r="M8" s="81">
         <v>6.4744999999999999</v>
       </c>
-      <c r="L8" s="80">
+      <c r="N8" s="81">
         <v>0.36609999999999998</v>
       </c>
-      <c r="M8" s="80">
+      <c r="O8" s="81">
         <v>5.7979000000000003</v>
       </c>
-      <c r="N8" s="80">
+      <c r="P8" s="81">
         <v>0.30930000000000002</v>
       </c>
-      <c r="O8" s="79"/>
-      <c r="P8" s="78">
+      <c r="Q8" s="80"/>
+      <c r="R8" s="79">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="77">
+      <c r="C9" s="78">
         <v>30</v>
       </c>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="78">
+      <c r="E9" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="79">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F9" s="78">
+      <c r="G9" s="79">
         <v>500</v>
       </c>
-      <c r="G9" s="78">
+      <c r="H9" s="79">
         <v>8</v>
       </c>
-      <c r="H9" s="78">
-        <f>80%*F9</f>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79">
+        <f>80%*G9</f>
         <v>400</v>
       </c>
-      <c r="I9" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="79"/>
-      <c r="K9" s="80">
+      <c r="K9" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="80"/>
+      <c r="M9" s="81">
         <v>8.9992000000000001</v>
       </c>
-      <c r="L9" s="80">
+      <c r="N9" s="81">
         <v>0.50509999999999999</v>
       </c>
-      <c r="M9" s="80">
+      <c r="O9" s="81">
         <v>7.8844000000000003</v>
       </c>
-      <c r="N9" s="80">
+      <c r="P9" s="81">
         <v>0.46489999999999998</v>
       </c>
-      <c r="O9" s="79"/>
-      <c r="P9" s="78">
+      <c r="Q9" s="80"/>
+      <c r="R9" s="79">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="77">
+      <c r="C10" s="78">
         <v>50</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="78">
-        <v>1E-4</v>
-      </c>
-      <c r="F10" s="78">
+      <c r="E10" s="78" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="79">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="79">
         <v>400</v>
       </c>
-      <c r="G10" s="78">
+      <c r="H10" s="79">
         <v>8</v>
       </c>
-      <c r="H10" s="78">
-        <f>80%*F10</f>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79">
+        <f>80%*G10</f>
         <v>320</v>
       </c>
-      <c r="I10" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="79"/>
-      <c r="K10" s="80">
+      <c r="K10" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="80"/>
+      <c r="M10" s="81">
         <v>4.3776000000000002</v>
       </c>
-      <c r="L10" s="80">
+      <c r="N10" s="81">
         <v>0.25919999999999999</v>
       </c>
-      <c r="M10" s="80">
+      <c r="O10" s="81">
         <v>4.6177000000000001</v>
       </c>
-      <c r="N10" s="80">
+      <c r="P10" s="81">
         <v>0.25719999999999998</v>
       </c>
-      <c r="O10" s="79"/>
-      <c r="P10" s="78">
+      <c r="Q10" s="80"/>
+      <c r="R10" s="79">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
+    <row r="11" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="78">
+        <v>50</v>
+      </c>
+      <c r="D11" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="79">
+        <v>1E-4</v>
+      </c>
+      <c r="G11" s="79">
+        <v>400</v>
+      </c>
+      <c r="H11" s="79">
+        <v>8</v>
+      </c>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79">
+        <f>80%*G11</f>
+        <v>320</v>
+      </c>
+      <c r="K11" s="79" t="s">
+        <v>6</v>
+      </c>
       <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="79"/>
-      <c r="P11" s="78"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="80"/>
+      <c r="M11" s="81">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="N11" s="81">
+        <v>0.27189999999999998</v>
+      </c>
+      <c r="O11" s="81">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="P11" s="81">
+        <v>0.26069999999999999</v>
+      </c>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="79">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="82" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="78">
+        <v>50</v>
+      </c>
+      <c r="D12" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="79">
+        <v>1E-4</v>
+      </c>
+      <c r="G12" s="79">
+        <v>200</v>
+      </c>
+      <c r="H12" s="79">
+        <v>16</v>
+      </c>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79">
+        <f>INT(C12/H12)*G12</f>
+        <v>600</v>
+      </c>
+      <c r="K12" s="79" t="s">
+        <v>6</v>
+      </c>
       <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="78"/>
+      <c r="M12" s="81">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="N12" s="81">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="O12" s="81">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="P12" s="81">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="79">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="78">
+        <v>50</v>
+      </c>
+      <c r="D13" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="69">
+        <v>1E-4</v>
+      </c>
+      <c r="G13" s="69">
+        <v>100</v>
+      </c>
+      <c r="H13" s="69">
+        <v>8</v>
+      </c>
+      <c r="I13" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="69">
+        <f>INT(C13/H13)*G13</f>
+        <v>600</v>
+      </c>
+      <c r="K13" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="80"/>
+      <c r="M13" s="81">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N13" s="81">
+        <v>0.43169999999999997</v>
+      </c>
+      <c r="O13" s="81">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P13" s="81">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="79">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="82"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="81"/>
+      <c r="P14" s="81"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="79"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="82"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="79"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="82"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="79"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="82"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="79"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="82"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="81"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="79"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="82"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="81"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="J5:J12"/>
-    <mergeCell ref="O5:O12"/>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="L5:L19"/>
+    <mergeCell ref="Q5:Q19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add - el decay steps es un hiperparametro importante para las métricas
se guarda un modelo 5 que usa norm z-core y un decay steps igual a la cantidad de épocas totales.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8C31EA-CCBD-49B8-BE08-A5023E311231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34707E4F-C047-4BD8-86AC-8C40DA5A4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="4440" windowWidth="21600" windowHeight="9075" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="1365" yWindow="4335" windowWidth="26280" windowHeight="8355" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="75">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>unet_model_decay_coseno_with_normalization_minmax_3.keras</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_zcore_4.keras</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_zcore_5.keras</t>
   </si>
 </sst>
 </file>
@@ -503,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -701,12 +707,24 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -728,22 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1113,24 +1116,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1919,10 +1922,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="74" t="s">
+      <c r="Q23" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="75"/>
+      <c r="R23" s="79"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1962,8 +1965,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="76"/>
-      <c r="R24" s="75"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="79"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2003,8 +2006,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="75"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="79"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2044,8 +2047,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="76"/>
-      <c r="R26" s="75"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="79"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2085,8 +2088,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="75"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="79"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2126,8 +2129,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="75"/>
+      <c r="Q28" s="80"/>
+      <c r="R28" s="79"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2167,8 +2170,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="76"/>
-      <c r="R29" s="75"/>
+      <c r="Q29" s="80"/>
+      <c r="R29" s="79"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2208,8 +2211,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="76"/>
-      <c r="R30" s="75"/>
+      <c r="Q30" s="80"/>
+      <c r="R30" s="79"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2249,8 +2252,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="76"/>
-      <c r="R31" s="75"/>
+      <c r="Q31" s="80"/>
+      <c r="R31" s="79"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2290,8 +2293,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="76"/>
-      <c r="R32" s="75"/>
+      <c r="Q32" s="80"/>
+      <c r="R32" s="79"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2331,8 +2334,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="76"/>
-      <c r="R33" s="75"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="79"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2372,8 +2375,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="76"/>
-      <c r="R34" s="75"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="79"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2413,8 +2416,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="76"/>
-      <c r="R35" s="75"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="79"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2454,8 +2457,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="76"/>
-      <c r="R36" s="75"/>
+      <c r="Q36" s="80"/>
+      <c r="R36" s="79"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2495,21 +2498,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="76"/>
-      <c r="R37" s="75"/>
+      <c r="Q37" s="80"/>
+      <c r="R37" s="79"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="73"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -2986,8 +2989,8 @@
   </sheetPr>
   <dimension ref="B3:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,557 +3009,614 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="71"/>
+      <c r="C3" s="75"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="70" t="s">
+      <c r="F5" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="70" t="s">
+      <c r="I5" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="J5" s="70" t="s">
+      <c r="J5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="70" t="s">
+      <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="77"/>
-      <c r="M5" s="70" t="s">
+      <c r="L5" s="81"/>
+      <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="70" t="s">
+      <c r="N5" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="70" t="s">
+      <c r="O5" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="70" t="s">
+      <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="70" t="s">
+      <c r="Q5" s="81"/>
+      <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="78">
+      <c r="C6" s="70">
         <v>30</v>
       </c>
-      <c r="D6" s="78" t="s">
+      <c r="D6" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79">
-        <v>1E-4</v>
-      </c>
-      <c r="G6" s="79">
+      <c r="E6" s="70"/>
+      <c r="F6" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="71">
         <v>500</v>
       </c>
-      <c r="H6" s="79">
+      <c r="H6" s="71">
         <v>8</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79">
-        <f>80%*G6</f>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71">
+        <f t="shared" ref="J6:J11" si="0">80%*G6</f>
         <v>400</v>
       </c>
-      <c r="K6" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="80"/>
-      <c r="M6" s="81">
+      <c r="K6" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="82"/>
+      <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
-      <c r="N6" s="81">
+      <c r="N6" s="72">
         <v>0.18490000000000001</v>
       </c>
-      <c r="O6" s="81">
+      <c r="O6" s="72">
         <v>7.4399999999999994E-2</v>
       </c>
-      <c r="P6" s="81">
+      <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="79">
+      <c r="Q6" s="82"/>
+      <c r="R6" s="71">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="70">
         <v>30</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="78" t="s">
+      <c r="E7" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="79">
-        <v>1E-4</v>
-      </c>
-      <c r="G7" s="79">
+      <c r="F7" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="71">
         <v>500</v>
       </c>
-      <c r="H7" s="79">
+      <c r="H7" s="71">
         <v>8</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79">
-        <f>80%*G7</f>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71">
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="K7" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="80"/>
-      <c r="M7" s="81">
+      <c r="K7" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="82"/>
+      <c r="M7" s="72">
         <v>4.5789</v>
       </c>
-      <c r="N7" s="81">
+      <c r="N7" s="72">
         <v>0.25600000000000001</v>
       </c>
-      <c r="O7" s="81">
+      <c r="O7" s="72">
         <v>4.1780999999999997</v>
       </c>
-      <c r="P7" s="81">
+      <c r="P7" s="72">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="79">
+      <c r="Q7" s="82"/>
+      <c r="R7" s="71">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="78">
+      <c r="C8" s="70">
         <v>30</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="78" t="s">
+      <c r="E8" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="79">
-        <v>1E-4</v>
-      </c>
-      <c r="G8" s="79">
+      <c r="F8" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="71">
         <v>410</v>
       </c>
-      <c r="H8" s="79">
+      <c r="H8" s="71">
         <v>8</v>
       </c>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79">
-        <f>80%*G8</f>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71">
+        <f t="shared" si="0"/>
         <v>328</v>
       </c>
-      <c r="K8" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="80"/>
-      <c r="M8" s="81">
+      <c r="K8" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="82"/>
+      <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
-      <c r="N8" s="81">
+      <c r="N8" s="72">
         <v>0.36609999999999998</v>
       </c>
-      <c r="O8" s="81">
+      <c r="O8" s="72">
         <v>5.7979000000000003</v>
       </c>
-      <c r="P8" s="81">
+      <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="79">
+      <c r="Q8" s="82"/>
+      <c r="R8" s="71">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="78">
+      <c r="C9" s="70">
         <v>30</v>
       </c>
-      <c r="D9" s="78" t="s">
+      <c r="D9" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="79">
+      <c r="F9" s="71">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G9" s="79">
+      <c r="G9" s="71">
         <v>500</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="71">
         <v>8</v>
       </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79">
-        <f>80%*G9</f>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71">
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="K9" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" s="80"/>
-      <c r="M9" s="81">
+      <c r="K9" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="82"/>
+      <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
-      <c r="N9" s="81">
+      <c r="N9" s="72">
         <v>0.50509999999999999</v>
       </c>
-      <c r="O9" s="81">
+      <c r="O9" s="72">
         <v>7.8844000000000003</v>
       </c>
-      <c r="P9" s="81">
+      <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="80"/>
-      <c r="R9" s="79">
+      <c r="Q9" s="82"/>
+      <c r="R9" s="71">
         <v>131</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="78">
+      <c r="C10" s="70">
         <v>50</v>
       </c>
-      <c r="D10" s="78" t="s">
+      <c r="D10" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="79">
-        <v>1E-4</v>
-      </c>
-      <c r="G10" s="79">
+      <c r="F10" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="71">
         <v>400</v>
       </c>
-      <c r="H10" s="79">
+      <c r="H10" s="71">
         <v>8</v>
       </c>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79">
-        <f>80%*G10</f>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71">
+        <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="K10" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="80"/>
-      <c r="M10" s="81">
+      <c r="K10" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="82"/>
+      <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
-      <c r="N10" s="81">
+      <c r="N10" s="72">
         <v>0.25919999999999999</v>
       </c>
-      <c r="O10" s="81">
+      <c r="O10" s="72">
         <v>4.6177000000000001</v>
       </c>
-      <c r="P10" s="81">
+      <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="80"/>
-      <c r="R10" s="79">
+      <c r="Q10" s="82"/>
+      <c r="R10" s="71">
         <v>179</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="78">
+      <c r="C11" s="70">
         <v>50</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="78" t="s">
+      <c r="E11" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="79">
-        <v>1E-4</v>
-      </c>
-      <c r="G11" s="79">
+      <c r="F11" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G11" s="71">
         <v>400</v>
       </c>
-      <c r="H11" s="79">
+      <c r="H11" s="71">
         <v>8</v>
       </c>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79">
-        <f>80%*G11</f>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71">
+        <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="K11" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="80"/>
-      <c r="M11" s="81">
+      <c r="K11" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="82"/>
+      <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="N11" s="81">
+      <c r="N11" s="72">
         <v>0.27189999999999998</v>
       </c>
-      <c r="O11" s="81">
+      <c r="O11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="P11" s="81">
+      <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="80"/>
-      <c r="R11" s="79">
+      <c r="Q11" s="82"/>
+      <c r="R11" s="71">
         <v>182</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="78">
+      <c r="C12" s="70">
         <v>50</v>
       </c>
-      <c r="D12" s="78" t="s">
+      <c r="D12" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="78" t="s">
+      <c r="E12" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="79">
-        <v>1E-4</v>
-      </c>
-      <c r="G12" s="79">
+      <c r="F12" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G12" s="71">
         <v>200</v>
       </c>
-      <c r="H12" s="79">
+      <c r="H12" s="71">
         <v>16</v>
       </c>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79">
+      <c r="I12" s="71"/>
+      <c r="J12" s="71">
         <f>INT(C12/H12)*G12</f>
         <v>600</v>
       </c>
-      <c r="K12" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" s="80"/>
-      <c r="M12" s="81">
+      <c r="K12" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="82"/>
+      <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="N12" s="81">
+      <c r="N12" s="72">
         <v>0.38500000000000001</v>
       </c>
-      <c r="O12" s="81">
+      <c r="O12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="P12" s="81">
+      <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="80"/>
-      <c r="R12" s="79">
+      <c r="Q12" s="82"/>
+      <c r="R12" s="71">
         <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="78">
+      <c r="C13" s="70">
         <v>50</v>
       </c>
-      <c r="D13" s="78" t="s">
+      <c r="D13" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="69">
-        <v>1E-4</v>
-      </c>
-      <c r="G13" s="69">
+      <c r="F13" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G13" s="71">
         <v>100</v>
       </c>
-      <c r="H13" s="69">
+      <c r="H13" s="71">
         <v>8</v>
       </c>
-      <c r="I13" s="69">
+      <c r="I13" s="71">
         <v>0.1</v>
       </c>
-      <c r="J13" s="69">
+      <c r="J13" s="71">
         <f>INT(C13/H13)*G13</f>
         <v>600</v>
       </c>
-      <c r="K13" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="80"/>
-      <c r="M13" s="81">
+      <c r="K13" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="82"/>
+      <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N13" s="81">
+      <c r="N13" s="72">
         <v>0.43169999999999997</v>
       </c>
-      <c r="O13" s="81">
+      <c r="O13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="P13" s="81">
+      <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="80"/>
-      <c r="R13" s="79">
+      <c r="Q13" s="82"/>
+      <c r="R13" s="71">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="82"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="80"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="80"/>
-      <c r="R14" s="79"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="82"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="80"/>
-      <c r="R15" s="79"/>
+    <row r="14" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="70">
+        <v>50</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="G14" s="71">
+        <v>700</v>
+      </c>
+      <c r="H14" s="71">
+        <v>8</v>
+      </c>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71">
+        <f>INT(C14/H14)*G14</f>
+        <v>4200</v>
+      </c>
+      <c r="K14" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="82"/>
+      <c r="M14" s="72">
+        <v>1.1584000000000001</v>
+      </c>
+      <c r="N14" s="72">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="O14" s="72">
+        <v>3.7222</v>
+      </c>
+      <c r="P14" s="72">
+        <v>0.1976</v>
+      </c>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="71">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="70">
+        <v>50</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="71">
+        <v>1E-3</v>
+      </c>
+      <c r="G15" s="71">
+        <v>300</v>
+      </c>
+      <c r="H15" s="71">
+        <v>8</v>
+      </c>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71">
+        <v>300</v>
+      </c>
+      <c r="K15" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="82"/>
+      <c r="M15" s="72">
+        <v>0.17349999999999999</v>
+      </c>
+      <c r="N15" s="72">
+        <v>0.01</v>
+      </c>
+      <c r="O15" s="72">
+        <v>3.2698</v>
+      </c>
+      <c r="P15" s="72">
+        <v>0.19939999999999999</v>
+      </c>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="71">
+        <v>118</v>
+      </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="82"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="80"/>
-      <c r="R16" s="79"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="82"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="71"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="82"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="79"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="71"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="82"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="79"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="72"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="71"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="82"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="80"/>
-      <c r="R19" s="79"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="72"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Add - nuevo mejor modelo sin decaimiento del LR
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34707E4F-C047-4BD8-86AC-8C40DA5A4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA125E09-3038-4BF6-92B7-87488A6CC262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="4335" windowWidth="26280" windowHeight="8355" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="930" yWindow="4485" windowWidth="26280" windowHeight="8355" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="77">
   <si>
     <t>MODELO U-NET: FULL SIGNALS</t>
   </si>
@@ -283,6 +283,12 @@
   <si>
     <t>unet_model_decay_coseno_with_normalization_zcore_5.keras</t>
   </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_zcore_6.keras</t>
+  </si>
+  <si>
+    <t>unet_model_decay_coseno_with_normalization_zcore_7.keras</t>
+  </si>
 </sst>
 </file>
 
@@ -292,7 +298,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +352,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -748,6 +760,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,7 +1112,7 @@
   </sheetPr>
   <dimension ref="B2:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD32"/>
     </sheetView>
   </sheetViews>
@@ -2989,8 +3007,8 @@
   </sheetPr>
   <dimension ref="B3:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,50 +3128,50 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="70">
+      <c r="C7" s="6">
         <v>30</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="71">
-        <v>1E-4</v>
-      </c>
-      <c r="G7" s="71">
+      <c r="F7" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="6">
         <v>500</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="6">
         <v>8</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="K7" s="71" t="s">
+      <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L7" s="82"/>
-      <c r="M7" s="72">
+      <c r="M7" s="83">
         <v>4.5789</v>
       </c>
-      <c r="N7" s="72">
+      <c r="N7" s="83">
         <v>0.25600000000000001</v>
       </c>
-      <c r="O7" s="72">
+      <c r="O7" s="83">
         <v>4.1780999999999997</v>
       </c>
-      <c r="P7" s="72">
+      <c r="P7" s="83">
         <v>0.2122</v>
       </c>
       <c r="Q7" s="82"/>
-      <c r="R7" s="71">
+      <c r="R7" s="6">
         <v>120</v>
       </c>
     </row>
@@ -3496,89 +3514,143 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="70">
+      <c r="C15" s="6">
         <v>50</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="6">
         <v>1E-3</v>
       </c>
-      <c r="G15" s="71">
+      <c r="G15" s="6">
         <v>300</v>
       </c>
-      <c r="H15" s="71">
+      <c r="H15" s="6">
         <v>8</v>
       </c>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="K15" s="71" t="s">
+      <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L15" s="82"/>
-      <c r="M15" s="72">
+      <c r="M15" s="83">
         <v>0.17349999999999999</v>
       </c>
-      <c r="N15" s="72">
+      <c r="N15" s="83">
         <v>0.01</v>
       </c>
-      <c r="O15" s="72">
+      <c r="O15" s="83">
         <v>3.2698</v>
       </c>
-      <c r="P15" s="72">
+      <c r="P15" s="83">
         <v>0.19939999999999999</v>
       </c>
       <c r="Q15" s="82"/>
-      <c r="R15" s="71">
+      <c r="R15" s="6">
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="73"/>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
+    <row r="16" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="70">
+        <v>50</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="71">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G16" s="71">
+        <v>300</v>
+      </c>
+      <c r="H16" s="71">
+        <v>8</v>
+      </c>
       <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
+      <c r="J16" s="71">
+        <v>300</v>
+      </c>
+      <c r="K16" s="71" t="s">
+        <v>6</v>
+      </c>
       <c r="L16" s="82"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
+      <c r="M16" s="72">
+        <v>8.2579999999999991</v>
+      </c>
+      <c r="N16" s="72">
+        <v>0.4854</v>
+      </c>
+      <c r="O16" s="72">
+        <v>7.8304</v>
+      </c>
+      <c r="P16" s="72">
+        <v>0.47870000000000001</v>
+      </c>
       <c r="Q16" s="82"/>
-      <c r="R16" s="71"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="73"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
+      <c r="R16" s="71">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="6">
+        <v>50</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="G17" s="6">
+        <v>300</v>
+      </c>
+      <c r="H17" s="6">
+        <v>8</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
+        <v>300</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="L17" s="82"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
+      <c r="M17" s="83">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="N17" s="83">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O17" s="83">
+        <v>6.9500000000000006E-2</v>
+      </c>
+      <c r="P17" s="83">
+        <v>0.1825</v>
+      </c>
       <c r="Q17" s="82"/>
-      <c r="R17" s="71"/>
+      <c r="R17" s="6">
+        <v>132</v>
+      </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="73"/>
@@ -3624,6 +3696,7 @@
     <mergeCell ref="L5:L19"/>
     <mergeCell ref="Q5:Q19"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add - Obtención de matrrices complejas de señales originales
Se obtienes las coeficientes (matrices complejas) de señales PAM para tener los inputs adecuados para realizar una predicción de los coeficientes de la señal VSC. Estos archivos.mat se almacenan en una carpeta llamada inputs_coeficientes en el directorio donde se encuentre el código fuente de la red neuronal. En el c´pdigo python se debe ingresar estos datos al modelo 7. este modelo no hace uso ni de decaimientos de LR y de una normalización determinada.
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA125E09-3038-4BF6-92B7-87488A6CC262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5A64BD-95A6-4532-9E22-A7241391A71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="4485" windowWidth="26280" windowHeight="8355" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
@@ -363,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +460,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -521,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -767,6 +773,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3005,10 +3012,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B3:R19"/>
+  <dimension ref="B3:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:K17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3607,7 +3614,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="84" t="s">
         <v>76</v>
       </c>
@@ -3651,8 +3658,9 @@
       <c r="R17" s="6">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="85"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="73"/>
       <c r="C18" s="70"/>
       <c r="D18" s="70"/>
@@ -3671,7 +3679,7 @@
       <c r="Q18" s="82"/>
       <c r="R18" s="71"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="73"/>
       <c r="C19" s="70"/>
       <c r="D19" s="70"/>

</xml_diff>

<commit_message>
Add - Predicción de coeficientes señal VSC
se transforma la matriz compleja estimada de VSC de formato .npy y tensor a formato .mat matriz compleja. El archivo nuevo .mat se almacena en una carpeta en el directorio de codigo_matlab
</commit_message>
<xml_diff>
--- a/Table_Comparative_Metrics_Models_Full_Signals.xlsx
+++ b/Table_Comparative_Metrics_Models_Full_Signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TT\Memoria\waveletycnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5A64BD-95A6-4532-9E22-A7241391A71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC3262-F42C-4B2D-85BA-81CF1B008B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="4485" windowWidth="26280" windowHeight="8355" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{437A2CD6-9E6E-4A6D-8312-6A31527F361A}"/>
   </bookViews>
   <sheets>
     <sheet name="full_signals - without decay" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
     <t>unet_model_decay_coseno_with_normalization_zcore_6.keras</t>
   </si>
   <si>
-    <t>unet_model_decay_coseno_with_normalization_zcore_7.keras</t>
+    <t>unet_model_7.keras</t>
   </si>
 </sst>
 </file>
@@ -743,6 +743,13 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,13 +774,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,24 +1141,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -1947,10 +1947,10 @@
       <c r="P23" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q23" s="78" t="s">
+      <c r="Q23" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="R23" s="79"/>
+      <c r="R23" s="82"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
@@ -1990,8 +1990,8 @@
       <c r="P24" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q24" s="80"/>
-      <c r="R24" s="79"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="82"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
@@ -2031,8 +2031,8 @@
       <c r="P25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q25" s="80"/>
-      <c r="R25" s="79"/>
+      <c r="Q25" s="83"/>
+      <c r="R25" s="82"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
@@ -2072,8 +2072,8 @@
       <c r="P26" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q26" s="80"/>
-      <c r="R26" s="79"/>
+      <c r="Q26" s="83"/>
+      <c r="R26" s="82"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="29" t="s">
@@ -2113,8 +2113,8 @@
       <c r="P27" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q27" s="80"/>
-      <c r="R27" s="79"/>
+      <c r="Q27" s="83"/>
+      <c r="R27" s="82"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
@@ -2154,8 +2154,8 @@
       <c r="P28" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q28" s="80"/>
-      <c r="R28" s="79"/>
+      <c r="Q28" s="83"/>
+      <c r="R28" s="82"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -2195,8 +2195,8 @@
       <c r="P29" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="80"/>
-      <c r="R29" s="79"/>
+      <c r="Q29" s="83"/>
+      <c r="R29" s="82"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
@@ -2236,8 +2236,8 @@
       <c r="P30" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q30" s="80"/>
-      <c r="R30" s="79"/>
+      <c r="Q30" s="83"/>
+      <c r="R30" s="82"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -2277,8 +2277,8 @@
       <c r="P31" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q31" s="80"/>
-      <c r="R31" s="79"/>
+      <c r="Q31" s="83"/>
+      <c r="R31" s="82"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="29" t="s">
@@ -2318,8 +2318,8 @@
       <c r="P32" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="Q32" s="80"/>
-      <c r="R32" s="79"/>
+      <c r="Q32" s="83"/>
+      <c r="R32" s="82"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
@@ -2359,8 +2359,8 @@
       <c r="P33" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="80"/>
-      <c r="R33" s="79"/>
+      <c r="Q33" s="83"/>
+      <c r="R33" s="82"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
@@ -2400,8 +2400,8 @@
       <c r="P34" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="79"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="82"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
@@ -2441,8 +2441,8 @@
       <c r="P35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="79"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="82"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
@@ -2482,8 +2482,8 @@
       <c r="P36" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q36" s="80"/>
-      <c r="R36" s="79"/>
+      <c r="Q36" s="83"/>
+      <c r="R36" s="82"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
@@ -2523,21 +2523,21 @@
       <c r="P37" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="Q37" s="80"/>
-      <c r="R37" s="79"/>
+      <c r="Q37" s="83"/>
+      <c r="R37" s="82"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="77" t="s">
+      <c r="B39" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="80"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="80"/>
+      <c r="H39" s="80"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
     </row>
     <row r="40" spans="2:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
@@ -3014,8 +3014,9 @@
   </sheetPr>
   <dimension ref="B3:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,10 +3035,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="78"/>
     </row>
     <row r="5" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
@@ -3070,7 +3071,7 @@
       <c r="K5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="81"/>
+      <c r="L5" s="84"/>
       <c r="M5" s="69" t="s">
         <v>7</v>
       </c>
@@ -3083,7 +3084,7 @@
       <c r="P5" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="81"/>
+      <c r="Q5" s="84"/>
       <c r="R5" s="69" t="s">
         <v>56</v>
       </c>
@@ -3116,7 +3117,7 @@
       <c r="K6" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="82"/>
+      <c r="L6" s="85"/>
       <c r="M6" s="72">
         <v>7.1400000000000005E-2</v>
       </c>
@@ -3129,7 +3130,7 @@
       <c r="P6" s="72">
         <v>0.16400000000000001</v>
       </c>
-      <c r="Q6" s="82"/>
+      <c r="Q6" s="85"/>
       <c r="R6" s="71">
         <v>116</v>
       </c>
@@ -3164,20 +3165,20 @@
       <c r="K7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="83">
+      <c r="L7" s="85"/>
+      <c r="M7" s="75">
         <v>4.5789</v>
       </c>
-      <c r="N7" s="83">
+      <c r="N7" s="75">
         <v>0.25600000000000001</v>
       </c>
-      <c r="O7" s="83">
+      <c r="O7" s="75">
         <v>4.1780999999999997</v>
       </c>
-      <c r="P7" s="83">
+      <c r="P7" s="75">
         <v>0.2122</v>
       </c>
-      <c r="Q7" s="82"/>
+      <c r="Q7" s="85"/>
       <c r="R7" s="6">
         <v>120</v>
       </c>
@@ -3212,7 +3213,7 @@
       <c r="K8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="82"/>
+      <c r="L8" s="85"/>
       <c r="M8" s="72">
         <v>6.4744999999999999</v>
       </c>
@@ -3225,7 +3226,7 @@
       <c r="P8" s="72">
         <v>0.30930000000000002</v>
       </c>
-      <c r="Q8" s="82"/>
+      <c r="Q8" s="85"/>
       <c r="R8" s="71">
         <v>116</v>
       </c>
@@ -3260,7 +3261,7 @@
       <c r="K9" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="82"/>
+      <c r="L9" s="85"/>
       <c r="M9" s="72">
         <v>8.9992000000000001</v>
       </c>
@@ -3273,7 +3274,7 @@
       <c r="P9" s="72">
         <v>0.46489999999999998</v>
       </c>
-      <c r="Q9" s="82"/>
+      <c r="Q9" s="85"/>
       <c r="R9" s="71">
         <v>131</v>
       </c>
@@ -3308,7 +3309,7 @@
       <c r="K10" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="82"/>
+      <c r="L10" s="85"/>
       <c r="M10" s="72">
         <v>4.3776000000000002</v>
       </c>
@@ -3321,7 +3322,7 @@
       <c r="P10" s="72">
         <v>0.25719999999999998</v>
       </c>
-      <c r="Q10" s="82"/>
+      <c r="Q10" s="85"/>
       <c r="R10" s="71">
         <v>179</v>
       </c>
@@ -3356,7 +3357,7 @@
       <c r="K11" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="82"/>
+      <c r="L11" s="85"/>
       <c r="M11" s="72">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -3369,7 +3370,7 @@
       <c r="P11" s="72">
         <v>0.26069999999999999</v>
       </c>
-      <c r="Q11" s="82"/>
+      <c r="Q11" s="85"/>
       <c r="R11" s="71">
         <v>182</v>
       </c>
@@ -3404,7 +3405,7 @@
       <c r="K12" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="82"/>
+      <c r="L12" s="85"/>
       <c r="M12" s="72">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -3417,7 +3418,7 @@
       <c r="P12" s="72">
         <v>0.39300000000000002</v>
       </c>
-      <c r="Q12" s="82"/>
+      <c r="Q12" s="85"/>
       <c r="R12" s="71">
         <v>89</v>
       </c>
@@ -3454,7 +3455,7 @@
       <c r="K13" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="82"/>
+      <c r="L13" s="85"/>
       <c r="M13" s="72">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -3467,7 +3468,7 @@
       <c r="P13" s="72">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q13" s="82"/>
+      <c r="Q13" s="85"/>
       <c r="R13" s="71">
         <v>44</v>
       </c>
@@ -3502,7 +3503,7 @@
       <c r="K14" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="82"/>
+      <c r="L14" s="85"/>
       <c r="M14" s="72">
         <v>1.1584000000000001</v>
       </c>
@@ -3515,13 +3516,13 @@
       <c r="P14" s="72">
         <v>0.1976</v>
       </c>
-      <c r="Q14" s="82"/>
+      <c r="Q14" s="85"/>
       <c r="R14" s="71">
         <v>305</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="76" t="s">
         <v>74</v>
       </c>
       <c r="C15" s="6">
@@ -3549,20 +3550,20 @@
       <c r="K15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="82"/>
-      <c r="M15" s="83">
+      <c r="L15" s="85"/>
+      <c r="M15" s="75">
         <v>0.17349999999999999</v>
       </c>
-      <c r="N15" s="83">
+      <c r="N15" s="75">
         <v>0.01</v>
       </c>
-      <c r="O15" s="83">
+      <c r="O15" s="75">
         <v>3.2698</v>
       </c>
-      <c r="P15" s="83">
+      <c r="P15" s="75">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q15" s="82"/>
+      <c r="Q15" s="85"/>
       <c r="R15" s="6">
         <v>118</v>
       </c>
@@ -3596,7 +3597,7 @@
       <c r="K16" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="82"/>
+      <c r="L16" s="85"/>
       <c r="M16" s="72">
         <v>8.2579999999999991</v>
       </c>
@@ -3609,13 +3610,13 @@
       <c r="P16" s="72">
         <v>0.47870000000000001</v>
       </c>
-      <c r="Q16" s="82"/>
+      <c r="Q16" s="85"/>
       <c r="R16" s="71">
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="84" t="s">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="76" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="6">
@@ -3635,30 +3636,28 @@
         <v>8</v>
       </c>
       <c r="I17" s="6"/>
-      <c r="J17" s="6">
-        <v>300</v>
-      </c>
+      <c r="J17" s="6"/>
       <c r="K17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="82"/>
-      <c r="M17" s="83">
+      <c r="L17" s="85"/>
+      <c r="M17" s="75">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="N17" s="83">
+      <c r="N17" s="75">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="O17" s="83">
+      <c r="O17" s="75">
         <v>6.9500000000000006E-2</v>
       </c>
-      <c r="P17" s="83">
+      <c r="P17" s="75">
         <v>0.1825</v>
       </c>
-      <c r="Q17" s="82"/>
+      <c r="Q17" s="85"/>
       <c r="R17" s="6">
         <v>132</v>
       </c>
-      <c r="S17" s="85"/>
+      <c r="S17" s="77"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="73"/>
@@ -3671,12 +3670,12 @@
       <c r="I18" s="71"/>
       <c r="J18" s="71"/>
       <c r="K18" s="71"/>
-      <c r="L18" s="82"/>
+      <c r="L18" s="85"/>
       <c r="M18" s="72"/>
       <c r="N18" s="72"/>
       <c r="O18" s="72"/>
       <c r="P18" s="72"/>
-      <c r="Q18" s="82"/>
+      <c r="Q18" s="85"/>
       <c r="R18" s="71"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3690,12 +3689,12 @@
       <c r="I19" s="71"/>
       <c r="J19" s="71"/>
       <c r="K19" s="71"/>
-      <c r="L19" s="82"/>
+      <c r="L19" s="85"/>
       <c r="M19" s="72"/>
       <c r="N19" s="72"/>
       <c r="O19" s="72"/>
       <c r="P19" s="72"/>
-      <c r="Q19" s="82"/>
+      <c r="Q19" s="85"/>
       <c r="R19" s="71"/>
     </row>
   </sheetData>

</xml_diff>